<commit_message>
Added some more functions
</commit_message>
<xml_diff>
--- a/EIS_TOOL.xlsx
+++ b/EIS_TOOL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BEAK_Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69902E8-4094-4860-B2FB-14961092B683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA329842-62C8-4531-B43B-20C5364E29E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C5D5763F-541F-4E53-AD9E-96294ACC5C82}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="211">
   <si>
     <t>EIS_TOOLKIT</t>
   </si>
@@ -537,6 +537,139 @@
   </si>
   <si>
     <t>Verwende einen Mexican hat filter filter auf das eingegebene Raster.</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>Agterberg-Cheng CI test (weights of evidence)</t>
+  </si>
+  <si>
+    <t>Classifier predict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classifier test </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuzzy overlay </t>
+  </si>
+  <si>
+    <t>Gradient boosting classifier</t>
+  </si>
+  <si>
+    <t>Gradient boosting regressor</t>
+  </si>
+  <si>
+    <t>Logistic regression</t>
+  </si>
+  <si>
+    <t>MLP classifier</t>
+  </si>
+  <si>
+    <t>MLP regressor</t>
+  </si>
+  <si>
+    <t>Random forest classifier</t>
+  </si>
+  <si>
+    <t>Random forest regressor</t>
+  </si>
+  <si>
+    <t>Regressor predict</t>
+  </si>
+  <si>
+    <t>Regressor test</t>
+  </si>
+  <si>
+    <t>Weights of evidence calculate responses</t>
+  </si>
+  <si>
+    <t>Weights of evidence calculate weights</t>
+  </si>
+  <si>
+    <t>Berechne eine 'und' Overlay-Operation mit unscharfer Logik.</t>
+  </si>
+  <si>
+    <t>Berechne eine 'oder' Overlay-Operation mit unscharfer Logik.</t>
+  </si>
+  <si>
+    <t>Berechne eine 'product' Overlay-Operation mit unscharfer Logik.</t>
+  </si>
+  <si>
+    <t>Berechne eine 'sum' Overlay-Operation mit unscharfer Logik.</t>
+  </si>
+  <si>
+    <t>Berechne eine 'gamma' Overlay-Operation mit unscharfer Logik.</t>
+  </si>
+  <si>
+    <t>numpy, eis_toolkit.exceptions, eis_toolkit.utilities.raster</t>
+  </si>
+  <si>
+    <t>fuzzy_overlay.py</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/master/eis_toolkit/prediction/fuzzy_overlay.py</t>
+  </si>
+  <si>
+    <t>and_overlay, _prepare_data_for_fuzzy_overlay</t>
+  </si>
+  <si>
+    <t>or_overlay, _prepare_data_for_fuzzy_overlay_prepare_data_for_fuzzy_overlay</t>
+  </si>
+  <si>
+    <t>product_overlay, _prepare_data_for_fuzzy_overlay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sum_overlay, _prepare_data_for_fuzzy_overlay</t>
+  </si>
+  <si>
+    <t>gamma_overlay, _prepare_data_for_fuzzy_overlay</t>
+  </si>
+  <si>
+    <t>cli.py</t>
+  </si>
+  <si>
+    <t>classifier_test_cli, eis_toolkit.evaluation.scoring -&gt; score_predictions, eis_toolkit.prediction.machine_learning_general -&gt; load_model, prepare_data_for_ml, reshape_predictions, eis_toolkit.prediction.machine_learning_predict -&gt; predict_classifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teste das trainierte maschinelle Lernklassifikationsmodell, indem du Vorhersagen triffst und bewertest.
+</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/46cc25c1de69ee8b66c7a752ba5dfa47d33847c1/eis_toolkit/cli.py#L2797</t>
+  </si>
+  <si>
+    <t>Nicht gefunden?</t>
+  </si>
+  <si>
+    <t>weights_of_evidence.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> agterberg_cheng_CI_test, _calculate_nr_of_deposit_pixels, </t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/46cc25c1de69ee8b66c7a752ba5dfa47d33847c1/eis_toolkit/prediction/weights_of_evidence.py#L253</t>
+  </si>
+  <si>
+    <t>Führe den Konditionalunabhängigkeitstest durch, der von Agterberg-Cheng (2002) vorgestellt wurde.</t>
+  </si>
+  <si>
+    <t>numpy, pandas</t>
+  </si>
+  <si>
+    <t>gradient_boosting.py</t>
+  </si>
+  <si>
+    <t>Trainiere und optional validiere ein Gradient Boosting Klassifikationsmodell mit Sklearn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GradientBoostingRegressor, _train_and_validate_sklearn_model, </t>
+  </si>
+  <si>
+    <t>numpy, pandas, sklearn.ensemble -&gt; GradientBoostingClassifier, GradientBoostingRegressor,  eis_toolkit.exceptions -&gt; InvalidParameterValueException, eis_toolkit.prediction.machine_learning_general -&gt; _train_and_validate_sklearn_model</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/46cc25c1de69ee8b66c7a752ba5dfa47d33847c1/eis_toolkit/prediction/gradient_boosting.py#L14</t>
   </si>
 </sst>
 </file>
@@ -881,7 +1014,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -945,6 +1078,147 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -973,13 +1247,49 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -997,10 +1307,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1014,6 +1336,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1023,6 +1357,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1039,15 +1379,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1056,6 +1390,39 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1072,232 +1439,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1639,60 +1781,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A14118C-3B2E-47A8-AB52-8BB0F98EF7A4}">
-  <dimension ref="A1:Q68"/>
+  <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:A68"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" style="100" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" style="66" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5546875" style="67" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" style="83" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44" style="24" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" style="30" customWidth="1"/>
     <col min="6" max="6" width="31" style="22" customWidth="1"/>
     <col min="7" max="7" width="102.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="78"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="101" t="s">
+      <c r="E3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="105" t="s">
+      <c r="F3" s="41" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -1700,19 +1844,19 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="102" t="s">
+      <c r="C4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="106" t="s">
+      <c r="E4" s="42" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="8" t="s">
@@ -1723,60 +1867,60 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="85" t="s">
+      <c r="A5" s="71"/>
+      <c r="B5" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="107" t="s">
+      <c r="E5" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="113" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="107" t="s">
+      <c r="A6" s="71"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="47"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="114"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="107" t="s">
+      <c r="A7" s="71"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="47"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="114"/>
     </row>
     <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="B8" s="88" t="s">
+      <c r="A8" s="71"/>
+      <c r="B8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="103" t="s">
+      <c r="C8" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="108" t="s">
+      <c r="E8" s="44" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="20" t="s">
@@ -1787,17 +1931,17 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="89" t="s">
+      <c r="A9" s="71"/>
+      <c r="B9" s="33" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="73" t="s">
+      <c r="D9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="107" t="s">
+      <c r="E9" s="43" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="21" t="s">
@@ -1808,17 +1952,17 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="88" t="s">
+      <c r="A10" s="71"/>
+      <c r="B10" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="103" t="s">
+      <c r="C10" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="108" t="s">
+      <c r="E10" s="44" t="s">
         <v>32</v>
       </c>
       <c r="F10" s="20" t="s">
@@ -1829,23 +1973,23 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
-      <c r="B11" s="90" t="s">
+      <c r="A11" s="71"/>
+      <c r="B11" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="107" t="s">
+      <c r="E11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="G11" s="115" t="s">
         <v>46</v>
       </c>
       <c r="H11" s="3"/>
@@ -1860,15 +2004,15 @@
       <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="90"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="107" t="s">
+      <c r="A12" s="71"/>
+      <c r="B12" s="103"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="48"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="115"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1881,15 +2025,15 @@
       <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="90"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="107" t="s">
+      <c r="A13" s="71"/>
+      <c r="B13" s="103"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="48"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="115"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1902,15 +2046,15 @@
       <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="90"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="107" t="s">
+      <c r="A14" s="71"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="48"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="115"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1923,15 +2067,15 @@
       <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="90"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="107" t="s">
+      <c r="A15" s="71"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="48"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="115"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1944,15 +2088,15 @@
       <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="90"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="107" t="s">
+      <c r="A16" s="71"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="48"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="115"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -1965,15 +2109,15 @@
       <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="90"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="107" t="s">
+      <c r="A17" s="71"/>
+      <c r="B17" s="103"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="48"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="115"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1986,15 +2130,15 @@
       <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="90"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="107" t="s">
+      <c r="A18" s="71"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="101"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="48"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="115"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -2007,183 +2151,183 @@
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
+      <c r="A19" s="71"/>
       <c r="B19" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="75" t="s">
+      <c r="D19" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="108" t="s">
+      <c r="E19" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="38" t="s">
+      <c r="F19" s="97" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="98" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
+      <c r="A20" s="71"/>
       <c r="B20" s="92"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="108" t="s">
+      <c r="C20" s="95"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="98"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
+      <c r="A21" s="71"/>
       <c r="B21" s="92"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="108" t="s">
+      <c r="C21" s="95"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="39"/>
+      <c r="F21" s="97"/>
+      <c r="G21" s="98"/>
     </row>
     <row r="22" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
+      <c r="A22" s="71"/>
       <c r="B22" s="93"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="108" t="s">
+      <c r="C22" s="96"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
+      <c r="F22" s="97"/>
+      <c r="G22" s="98"/>
     </row>
     <row r="23" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="90" t="s">
+      <c r="A23" s="71"/>
+      <c r="B23" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="74" t="s">
+      <c r="D23" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="107" t="s">
+      <c r="E23" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="42" t="s">
+      <c r="F23" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="44" t="s">
+      <c r="G23" s="107" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
-      <c r="B24" s="90"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="107" t="s">
+      <c r="A24" s="71"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="101"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="44"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="107"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
-      <c r="B25" s="90"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="107" t="s">
+      <c r="A25" s="71"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="99"/>
+      <c r="E25" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="42"/>
-      <c r="G25" s="44"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="107"/>
     </row>
     <row r="26" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="24"/>
-      <c r="B26" s="90"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="107" t="s">
+      <c r="A26" s="71"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="101"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="42"/>
-      <c r="G26" s="44"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="107"/>
     </row>
     <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="25"/>
-      <c r="B27" s="94"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="109" t="s">
+      <c r="A27" s="72"/>
+      <c r="B27" s="104"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="43"/>
-      <c r="G27" s="45"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="108"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="95" t="s">
+      <c r="B28" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="79" t="s">
+      <c r="D28" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="110" t="s">
+      <c r="E28" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="49" t="s">
+      <c r="F28" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="51" t="s">
+      <c r="G28" s="120" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="24"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="80"/>
-      <c r="E29" s="111" t="s">
+      <c r="A29" s="71"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="110"/>
+      <c r="D29" s="124"/>
+      <c r="E29" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="50"/>
-      <c r="G29" s="52"/>
+      <c r="F29" s="119"/>
+      <c r="G29" s="121"/>
     </row>
     <row r="30" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="24"/>
-      <c r="B30" s="96"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="111" t="s">
+      <c r="A30" s="71"/>
+      <c r="B30" s="112"/>
+      <c r="C30" s="110"/>
+      <c r="D30" s="124"/>
+      <c r="E30" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="50"/>
-      <c r="G30" s="52"/>
+      <c r="F30" s="119"/>
+      <c r="G30" s="121"/>
     </row>
     <row r="31" spans="1:17" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="24"/>
-      <c r="B31" s="96"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="80"/>
-      <c r="E31" s="111" t="s">
+      <c r="A31" s="71"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="110"/>
+      <c r="D31" s="124"/>
+      <c r="E31" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="50"/>
-      <c r="G31" s="53"/>
+      <c r="F31" s="119"/>
+      <c r="G31" s="122"/>
     </row>
     <row r="32" spans="1:17" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="24"/>
-      <c r="B32" s="97" t="s">
+      <c r="A32" s="71"/>
+      <c r="B32" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C32" s="17" t="s">
@@ -2192,7 +2336,7 @@
       <c r="D32" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="112" t="s">
+      <c r="E32" s="47" t="s">
         <v>75</v>
       </c>
       <c r="F32" s="10" t="s">
@@ -2203,8 +2347,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24"/>
-      <c r="B33" s="97" t="s">
+      <c r="A33" s="71"/>
+      <c r="B33" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="17" t="s">
@@ -2213,7 +2357,7 @@
       <c r="D33" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="112" t="s">
+      <c r="E33" s="47" t="s">
         <v>75</v>
       </c>
       <c r="F33" s="10" t="s">
@@ -2224,136 +2368,136 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24"/>
-      <c r="B34" s="98" t="s">
+      <c r="A34" s="71"/>
+      <c r="B34" s="34" t="s">
         <v>80</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="81" t="s">
+      <c r="D34" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="82" t="s">
+      <c r="E34" s="116" t="s">
         <v>87</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="G34" s="57" t="s">
+      <c r="G34" s="117" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="24"/>
-      <c r="B35" s="98" t="s">
+      <c r="A35" s="71"/>
+      <c r="B35" s="34" t="s">
         <v>82</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="81" t="s">
+      <c r="D35" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="82"/>
+      <c r="E35" s="116"/>
       <c r="F35" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G35" s="57"/>
+      <c r="G35" s="117"/>
     </row>
     <row r="36" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="24"/>
-      <c r="B36" s="99" t="s">
+      <c r="A36" s="71"/>
+      <c r="B36" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="127" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="65" t="s">
+      <c r="D36" s="129" t="s">
         <v>90</v>
       </c>
-      <c r="E36" s="112" t="s">
+      <c r="E36" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="F36" s="58" t="s">
+      <c r="F36" s="125" t="s">
         <v>93</v>
       </c>
-      <c r="G36" s="59" t="s">
+      <c r="G36" s="126" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
-      <c r="B37" s="99"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="112" t="s">
+      <c r="A37" s="71"/>
+      <c r="B37" s="128"/>
+      <c r="C37" s="127"/>
+      <c r="D37" s="129"/>
+      <c r="E37" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="F37" s="58"/>
-      <c r="G37" s="59"/>
+      <c r="F37" s="125"/>
+      <c r="G37" s="126"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="24"/>
-      <c r="B38" s="99"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="112" t="s">
+      <c r="A38" s="71"/>
+      <c r="B38" s="128"/>
+      <c r="C38" s="127"/>
+      <c r="D38" s="129"/>
+      <c r="E38" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="58"/>
-      <c r="G38" s="59"/>
+      <c r="F38" s="125"/>
+      <c r="G38" s="126"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="24"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="112" t="s">
+      <c r="A39" s="71"/>
+      <c r="B39" s="128"/>
+      <c r="C39" s="127"/>
+      <c r="D39" s="129"/>
+      <c r="E39" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="F39" s="58"/>
-      <c r="G39" s="59"/>
+      <c r="F39" s="125"/>
+      <c r="G39" s="126"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="24"/>
-      <c r="B40" s="98" t="s">
+      <c r="A40" s="71"/>
+      <c r="B40" s="34" t="s">
         <v>96</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="81" t="s">
+      <c r="D40" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="E40" s="82" t="s">
+      <c r="E40" s="116" t="s">
         <v>103</v>
       </c>
-      <c r="F40" s="50" t="s">
+      <c r="F40" s="119" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="57" t="s">
+      <c r="G40" s="117" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="24"/>
-      <c r="B41" s="98" t="s">
+      <c r="A41" s="71"/>
+      <c r="B41" s="34" t="s">
         <v>99</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D41" s="81" t="s">
+      <c r="D41" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E41" s="82"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="57"/>
+      <c r="E41" s="116"/>
+      <c r="F41" s="119"/>
+      <c r="G41" s="117"/>
     </row>
     <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="24"/>
-      <c r="B42" s="97" t="s">
+      <c r="A42" s="71"/>
+      <c r="B42" s="35" t="s">
         <v>104</v>
       </c>
       <c r="C42" s="17" t="s">
@@ -2362,7 +2506,7 @@
       <c r="D42" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E42" s="112" t="s">
+      <c r="E42" s="47" t="s">
         <v>107</v>
       </c>
       <c r="F42" s="10" t="s">
@@ -2373,241 +2517,241 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="24"/>
-      <c r="B43" s="98" t="s">
+      <c r="A43" s="71"/>
+      <c r="B43" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="55" t="s">
+      <c r="C43" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="D43" s="82" t="s">
+      <c r="D43" s="116" t="s">
         <v>113</v>
       </c>
-      <c r="E43" s="82" t="s">
+      <c r="E43" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="F43" s="50" t="s">
+      <c r="F43" s="119" t="s">
         <v>112</v>
       </c>
-      <c r="G43" s="57" t="s">
+      <c r="G43" s="117" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="24"/>
-      <c r="B44" s="98" t="s">
+      <c r="A44" s="71"/>
+      <c r="B44" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C44" s="55"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="57"/>
+      <c r="C44" s="110"/>
+      <c r="D44" s="116"/>
+      <c r="E44" s="116"/>
+      <c r="F44" s="119"/>
+      <c r="G44" s="117"/>
     </row>
     <row r="45" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="24"/>
-      <c r="B45" s="99" t="s">
+      <c r="A45" s="71"/>
+      <c r="B45" s="128" t="s">
         <v>120</v>
       </c>
-      <c r="C45" s="56" t="s">
+      <c r="C45" s="127" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="60" t="s">
+      <c r="D45" s="138" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="113" t="s">
+      <c r="E45" s="143" t="s">
         <v>119</v>
       </c>
-      <c r="F45" s="58" t="s">
+      <c r="F45" s="125" t="s">
         <v>118</v>
       </c>
-      <c r="G45" s="59" t="s">
+      <c r="G45" s="126" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="24"/>
-      <c r="B46" s="99"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="113"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="59"/>
+      <c r="A46" s="71"/>
+      <c r="B46" s="128"/>
+      <c r="C46" s="127"/>
+      <c r="D46" s="139"/>
+      <c r="E46" s="143"/>
+      <c r="F46" s="125"/>
+      <c r="G46" s="126"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="24"/>
-      <c r="B47" s="99"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="113"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="59"/>
+      <c r="A47" s="71"/>
+      <c r="B47" s="128"/>
+      <c r="C47" s="127"/>
+      <c r="D47" s="139"/>
+      <c r="E47" s="143"/>
+      <c r="F47" s="125"/>
+      <c r="G47" s="126"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="24"/>
-      <c r="B48" s="99"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="61"/>
-      <c r="E48" s="113"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="59"/>
+      <c r="A48" s="71"/>
+      <c r="B48" s="128"/>
+      <c r="C48" s="127"/>
+      <c r="D48" s="139"/>
+      <c r="E48" s="143"/>
+      <c r="F48" s="125"/>
+      <c r="G48" s="126"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="24"/>
-      <c r="B49" s="99"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="62"/>
-      <c r="E49" s="113"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="59"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="128"/>
+      <c r="C49" s="127"/>
+      <c r="D49" s="140"/>
+      <c r="E49" s="143"/>
+      <c r="F49" s="125"/>
+      <c r="G49" s="126"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="24"/>
-      <c r="B50" s="96" t="s">
+      <c r="A50" s="71"/>
+      <c r="B50" s="112" t="s">
         <v>122</v>
       </c>
-      <c r="C50" s="55" t="s">
+      <c r="C50" s="110" t="s">
         <v>124</v>
       </c>
-      <c r="D50" s="63" t="s">
+      <c r="D50" s="141" t="s">
         <v>131</v>
       </c>
-      <c r="E50" s="111" t="s">
+      <c r="E50" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F50" s="50" t="s">
+      <c r="F50" s="119" t="s">
         <v>129</v>
       </c>
-      <c r="G50" s="57" t="s">
+      <c r="G50" s="117" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="24"/>
-      <c r="B51" s="96"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="111" t="s">
+      <c r="A51" s="71"/>
+      <c r="B51" s="112"/>
+      <c r="C51" s="110"/>
+      <c r="D51" s="142"/>
+      <c r="E51" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="F51" s="50"/>
-      <c r="G51" s="57"/>
+      <c r="F51" s="119"/>
+      <c r="G51" s="117"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="24"/>
-      <c r="B52" s="96"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="111" t="s">
+      <c r="A52" s="71"/>
+      <c r="B52" s="112"/>
+      <c r="C52" s="110"/>
+      <c r="D52" s="142"/>
+      <c r="E52" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F52" s="50"/>
-      <c r="G52" s="57"/>
+      <c r="F52" s="119"/>
+      <c r="G52" s="117"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="24"/>
-      <c r="B53" s="96"/>
-      <c r="C53" s="55"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="111" t="s">
+      <c r="A53" s="71"/>
+      <c r="B53" s="112"/>
+      <c r="C53" s="110"/>
+      <c r="D53" s="142"/>
+      <c r="E53" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="F53" s="50"/>
-      <c r="G53" s="57"/>
+      <c r="F53" s="119"/>
+      <c r="G53" s="117"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="24"/>
-      <c r="B54" s="96"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="64"/>
-      <c r="E54" s="111" t="s">
+      <c r="A54" s="71"/>
+      <c r="B54" s="112"/>
+      <c r="C54" s="110"/>
+      <c r="D54" s="142"/>
+      <c r="E54" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="F54" s="50"/>
-      <c r="G54" s="57"/>
+      <c r="F54" s="119"/>
+      <c r="G54" s="117"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="24"/>
-      <c r="B55" s="96"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="64"/>
-      <c r="E55" s="111" t="s">
+      <c r="A55" s="71"/>
+      <c r="B55" s="112"/>
+      <c r="C55" s="110"/>
+      <c r="D55" s="142"/>
+      <c r="E55" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="F55" s="50"/>
-      <c r="G55" s="57"/>
+      <c r="F55" s="119"/>
+      <c r="G55" s="117"/>
     </row>
     <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="24"/>
-      <c r="B56" s="96"/>
-      <c r="C56" s="55"/>
-      <c r="D56" s="64"/>
-      <c r="E56" s="111" t="s">
+      <c r="A56" s="71"/>
+      <c r="B56" s="112"/>
+      <c r="C56" s="110"/>
+      <c r="D56" s="142"/>
+      <c r="E56" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="F56" s="50"/>
-      <c r="G56" s="57"/>
+      <c r="F56" s="119"/>
+      <c r="G56" s="117"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="24"/>
-      <c r="B57" s="96"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="64"/>
-      <c r="E57" s="111" t="s">
+      <c r="A57" s="71"/>
+      <c r="B57" s="112"/>
+      <c r="C57" s="110"/>
+      <c r="D57" s="142"/>
+      <c r="E57" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="F57" s="50"/>
-      <c r="G57" s="57"/>
+      <c r="F57" s="119"/>
+      <c r="G57" s="117"/>
     </row>
     <row r="58" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="114"/>
-      <c r="B58" s="115"/>
-      <c r="C58" s="116"/>
-      <c r="D58" s="64"/>
+      <c r="A58" s="137"/>
+      <c r="B58" s="136"/>
+      <c r="C58" s="135"/>
+      <c r="D58" s="142"/>
       <c r="E58" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="F58" s="117"/>
-      <c r="G58" s="118"/>
+      <c r="F58" s="133"/>
+      <c r="G58" s="134"/>
     </row>
     <row r="59" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A59" s="119" t="s">
+      <c r="A59" s="130" t="s">
         <v>132</v>
       </c>
-      <c r="B59" s="122" t="s">
+      <c r="B59" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C59" s="123" t="s">
+      <c r="C59" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="D59" s="124" t="s">
+      <c r="D59" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="E59" s="124" t="s">
+      <c r="E59" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="F59" s="125" t="s">
+      <c r="F59" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="G59" s="126" t="s">
+      <c r="G59" s="52" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="120"/>
-      <c r="B60" s="132" t="s">
+      <c r="A60" s="131"/>
+      <c r="B60" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="C60" s="133" t="s">
+      <c r="C60" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="D60" s="134" t="s">
+      <c r="D60" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="E60" s="134" t="s">
+      <c r="E60" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="F60" s="135" t="s">
+      <c r="F60" s="61" t="s">
         <v>140</v>
       </c>
       <c r="G60" s="6" t="s">
@@ -2615,20 +2759,20 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A61" s="120"/>
-      <c r="B61" s="127" t="s">
+      <c r="A61" s="131"/>
+      <c r="B61" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="C61" s="128" t="s">
+      <c r="C61" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="D61" s="129" t="s">
+      <c r="D61" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="E61" s="129" t="s">
+      <c r="E61" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="F61" s="130" t="s">
+      <c r="F61" s="56" t="s">
         <v>144</v>
       </c>
       <c r="G61" s="7" t="s">
@@ -2636,20 +2780,20 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A62" s="120"/>
-      <c r="B62" s="132" t="s">
+      <c r="A62" s="131"/>
+      <c r="B62" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="C62" s="136" t="s">
+      <c r="C62" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="D62" s="134" t="s">
+      <c r="D62" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="E62" s="134" t="s">
+      <c r="E62" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="F62" s="135" t="s">
+      <c r="F62" s="61" t="s">
         <v>149</v>
       </c>
       <c r="G62" s="6" t="s">
@@ -2657,20 +2801,20 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A63" s="120"/>
-      <c r="B63" s="127" t="s">
+      <c r="A63" s="131"/>
+      <c r="B63" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="C63" s="131" t="s">
+      <c r="C63" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="D63" s="129" t="s">
+      <c r="D63" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="E63" s="129" t="s">
+      <c r="E63" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="F63" s="130" t="s">
+      <c r="F63" s="56" t="s">
         <v>152</v>
       </c>
       <c r="G63" s="7" t="s">
@@ -2678,20 +2822,20 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="120"/>
-      <c r="B64" s="132" t="s">
+      <c r="A64" s="131"/>
+      <c r="B64" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="C64" s="136" t="s">
+      <c r="C64" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="D64" s="134" t="s">
+      <c r="D64" s="60" t="s">
         <v>154</v>
       </c>
-      <c r="E64" s="134" t="s">
+      <c r="E64" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="F64" s="135" t="s">
+      <c r="F64" s="61" t="s">
         <v>161</v>
       </c>
       <c r="G64" s="6" t="s">
@@ -2699,20 +2843,20 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="120"/>
-      <c r="B65" s="127" t="s">
+      <c r="A65" s="131"/>
+      <c r="B65" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="C65" s="131" t="s">
+      <c r="C65" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="D65" s="129" t="s">
+      <c r="D65" s="55" t="s">
         <v>154</v>
       </c>
-      <c r="E65" s="129" t="s">
+      <c r="E65" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="F65" s="130" t="s">
+      <c r="F65" s="56" t="s">
         <v>155</v>
       </c>
       <c r="G65" s="7" t="s">
@@ -2720,20 +2864,20 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A66" s="120"/>
-      <c r="B66" s="132" t="s">
+      <c r="A66" s="131"/>
+      <c r="B66" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="C66" s="136" t="s">
+      <c r="C66" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="134" t="s">
+      <c r="D66" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="E66" s="134" t="s">
+      <c r="E66" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="F66" s="135" t="s">
+      <c r="F66" s="61" t="s">
         <v>162</v>
       </c>
       <c r="G66" s="6" t="s">
@@ -2741,49 +2885,266 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="120"/>
-      <c r="B67" s="127" t="s">
+      <c r="A67" s="131"/>
+      <c r="B67" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="C67" s="131" t="s">
+      <c r="C67" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="D67" s="129" t="s">
+      <c r="D67" s="55" t="s">
         <v>163</v>
       </c>
-      <c r="E67" s="129" t="s">
+      <c r="E67" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="F67" s="130" t="s">
+      <c r="F67" s="56" t="s">
         <v>164</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="121"/>
-      <c r="B68" s="137" t="s">
+    <row r="68" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="132"/>
+      <c r="B68" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="C68" s="138" t="s">
+      <c r="C68" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="D68" s="139" t="s">
+      <c r="D68" s="65" t="s">
         <v>145</v>
       </c>
-      <c r="E68" s="139" t="s">
+      <c r="E68" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="F68" s="140" t="s">
+      <c r="F68" s="66" t="s">
         <v>166</v>
       </c>
       <c r="G68" s="19" t="s">
         <v>148</v>
       </c>
     </row>
+    <row r="69" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>167</v>
+      </c>
+      <c r="B69" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="C69" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="D69" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="E69" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="F69" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B70" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="C70" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E70" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="F70" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="G70" s="23" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B71" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="C71" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F71" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B72" s="67" t="s">
+        <v>171</v>
+      </c>
+      <c r="C72" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="F72" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="G72" s="68" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B73" s="67"/>
+      <c r="C73" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D73" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="F73" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="G73" s="69"/>
+    </row>
+    <row r="74" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B74" s="67"/>
+      <c r="C74" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D74" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="F74" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="G74" s="69"/>
+    </row>
+    <row r="75" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B75" s="67"/>
+      <c r="C75" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="F75" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="G75" s="69"/>
+    </row>
+    <row r="76" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B76" s="67"/>
+      <c r="C76" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D76" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="F76" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="G76" s="69"/>
+    </row>
+    <row r="77" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="B77" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="D77" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="F77" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B78" s="36" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B79" s="36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B80" s="36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="36" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="36" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="36" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="36" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="36" t="s">
+        <v>182</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="57">
     <mergeCell ref="A59:A68"/>
     <mergeCell ref="F50:F58"/>
     <mergeCell ref="G50:G58"/>
@@ -2815,6 +3176,8 @@
     <mergeCell ref="F28:F31"/>
     <mergeCell ref="G28:G31"/>
     <mergeCell ref="D28:D31"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="F5:F7"/>
     <mergeCell ref="C28:C31"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="G5:G7"/>
@@ -2823,6 +3186,8 @@
     <mergeCell ref="B11:B18"/>
     <mergeCell ref="F11:F18"/>
     <mergeCell ref="G11:G18"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="G72:G76"/>
     <mergeCell ref="A4:A27"/>
     <mergeCell ref="A1:G2"/>
     <mergeCell ref="B5:B7"/>
@@ -2837,8 +3202,6 @@
     <mergeCell ref="C23:C27"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="F23:F27"/>
-    <mergeCell ref="G23:G27"/>
-    <mergeCell ref="F5:F7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G9" r:id="rId1" location="L7" xr:uid="{F521EE9C-24C9-46E9-9B83-619AF2EE0F94}"/>
@@ -2866,8 +3229,12 @@
     <hyperlink ref="G66" r:id="rId23" xr:uid="{8F487827-2DDE-47E6-B004-CCAB8E97B070}"/>
     <hyperlink ref="G67" r:id="rId24" xr:uid="{B82B31A8-30F5-43B7-83C3-3CD473DB8685}"/>
     <hyperlink ref="G68" r:id="rId25" xr:uid="{AC9E4A8A-1280-49A5-ADD4-39AF740EB6AB}"/>
+    <hyperlink ref="G72" r:id="rId26" xr:uid="{8701D585-6CCD-44A1-B91D-8DA741B79BD2}"/>
+    <hyperlink ref="G71" r:id="rId27" location="L2797" xr:uid="{AD5B641F-1BB5-4123-8009-DAD2333B61DB}"/>
+    <hyperlink ref="G69" r:id="rId28" location="L253" xr:uid="{1687F3D3-1E61-41F3-9F96-407ED35860EF}"/>
+    <hyperlink ref="G77" r:id="rId29" location="L14" xr:uid="{B1BCDC3D-AE1D-4597-B3CA-B22E52A94612}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed both the transform functions
</commit_message>
<xml_diff>
--- a/EIS_TOOL.xlsx
+++ b/EIS_TOOL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BEAK_Arbeit\EIS_TOOLKIT_FUNCTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E626B0B9-714E-43A0-9899-62F7F6EAD8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB22D8B-441A-430D-A7A2-C8513B317F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C5D5763F-541F-4E53-AD9E-96294ACC5C82}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="460">
   <si>
     <t>EIS_TOOLKIT</t>
   </si>
@@ -1497,9 +1497,6 @@
     <t>Single PLR transform</t>
   </si>
   <si>
-    <t>Perform a pivot logratio transformation on the selected column.</t>
-  </si>
-  <si>
     <t>alr.py</t>
   </si>
   <si>
@@ -1597,6 +1594,15 @@
   </si>
   <si>
     <t>Eine einzelne isometrische Logratios-Transformation auf die bereitgestellten Subkompositionen durchführen.</t>
+  </si>
+  <si>
+    <t>Führe eine Pivot-Logratio-Transformation auf der ausgewählten Spalte durch.</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/46cc25c1de69ee8b66c7a752ba5dfa47d33847c1/eis_toolkit/transformations/coda/plr.py#L60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single_plr_transform, _single_plr_transform,  _single_plr_transform_by_index, _calculate_plr_scaling_factor, </t>
   </si>
 </sst>
 </file>
@@ -2030,7 +2036,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -2325,16 +2331,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2345,27 +2360,213 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2385,200 +2586,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2922,10 +2931,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A14118C-3B2E-47A8-AB52-8BB0F98EF7A4}">
   <dimension ref="A1:Q123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C123" sqref="C123"/>
+      <selection pane="bottomLeft" activeCell="A116" sqref="A116:A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2940,24 +2949,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="129"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="139"/>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="130"/>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="132"/>
+      <c r="A2" s="140"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="142"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -2983,7 +2992,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="107" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -3006,50 +3015,50 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="105"/>
-      <c r="B5" s="133" t="s">
+      <c r="A5" s="108"/>
+      <c r="B5" s="143" t="s">
         <v>213</v>
       </c>
-      <c r="C5" s="136" t="s">
+      <c r="C5" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="139" t="s">
+      <c r="D5" s="149" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="153" t="s">
+      <c r="F5" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="154" t="s">
+      <c r="G5" s="163" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="105"/>
-      <c r="B6" s="134"/>
-      <c r="C6" s="137"/>
-      <c r="D6" s="140"/>
+      <c r="A6" s="108"/>
+      <c r="B6" s="144"/>
+      <c r="C6" s="147"/>
+      <c r="D6" s="150"/>
       <c r="E6" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="153"/>
-      <c r="G6" s="155"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="164"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="105"/>
-      <c r="B7" s="135"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="141"/>
+      <c r="A7" s="108"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="148"/>
+      <c r="D7" s="151"/>
       <c r="E7" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="153"/>
-      <c r="G7" s="155"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="105"/>
+      <c r="A8" s="108"/>
       <c r="B8" s="18" t="s">
         <v>21</v>
       </c>
@@ -3070,7 +3079,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="105"/>
+      <c r="A9" s="108"/>
       <c r="B9" s="19" t="s">
         <v>214</v>
       </c>
@@ -3091,7 +3100,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="105"/>
+      <c r="A10" s="108"/>
       <c r="B10" s="18" t="s">
         <v>215</v>
       </c>
@@ -3112,23 +3121,23 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="105"/>
-      <c r="B11" s="158" t="s">
+      <c r="A11" s="108"/>
+      <c r="B11" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="157" t="s">
+      <c r="C11" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="156" t="s">
+      <c r="D11" s="118" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="153" t="s">
+      <c r="F11" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="159" t="s">
+      <c r="G11" s="124" t="s">
         <v>45</v>
       </c>
       <c r="H11" s="2"/>
@@ -3143,15 +3152,15 @@
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="105"/>
-      <c r="B12" s="158"/>
-      <c r="C12" s="157"/>
-      <c r="D12" s="156"/>
+      <c r="A12" s="108"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="120"/>
+      <c r="D12" s="118"/>
       <c r="E12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="153"/>
-      <c r="G12" s="159"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="124"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -3164,15 +3173,15 @@
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="105"/>
-      <c r="B13" s="158"/>
-      <c r="C13" s="157"/>
-      <c r="D13" s="156"/>
+      <c r="A13" s="108"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="120"/>
+      <c r="D13" s="118"/>
       <c r="E13" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="153"/>
-      <c r="G13" s="159"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="124"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -3185,15 +3194,15 @@
       <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="105"/>
-      <c r="B14" s="158"/>
-      <c r="C14" s="157"/>
-      <c r="D14" s="156"/>
+      <c r="A14" s="108"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="118"/>
       <c r="E14" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="153"/>
-      <c r="G14" s="159"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="124"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -3206,15 +3215,15 @@
       <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="105"/>
-      <c r="B15" s="158"/>
-      <c r="C15" s="157"/>
-      <c r="D15" s="156"/>
+      <c r="A15" s="108"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="118"/>
       <c r="E15" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="153"/>
-      <c r="G15" s="159"/>
+      <c r="F15" s="122"/>
+      <c r="G15" s="124"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -3227,15 +3236,15 @@
       <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="105"/>
-      <c r="B16" s="158"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="156"/>
+      <c r="A16" s="108"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="118"/>
       <c r="E16" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="153"/>
-      <c r="G16" s="159"/>
+      <c r="F16" s="122"/>
+      <c r="G16" s="124"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -3248,15 +3257,15 @@
       <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="105"/>
-      <c r="B17" s="158"/>
-      <c r="C17" s="157"/>
-      <c r="D17" s="156"/>
+      <c r="A17" s="108"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="118"/>
       <c r="E17" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="153"/>
-      <c r="G17" s="159"/>
+      <c r="F17" s="122"/>
+      <c r="G17" s="124"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -3269,15 +3278,15 @@
       <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="105"/>
-      <c r="B18" s="158"/>
-      <c r="C18" s="157"/>
-      <c r="D18" s="156"/>
+      <c r="A18" s="108"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="118"/>
       <c r="E18" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="153"/>
-      <c r="G18" s="159"/>
+      <c r="F18" s="122"/>
+      <c r="G18" s="124"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -3290,182 +3299,182 @@
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="105"/>
-      <c r="B19" s="145" t="s">
+      <c r="A19" s="108"/>
+      <c r="B19" s="155" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="148" t="s">
+      <c r="C19" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="142" t="s">
+      <c r="D19" s="152" t="s">
         <v>46</v>
       </c>
       <c r="E19" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="151" t="s">
+      <c r="F19" s="161" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="152" t="s">
+      <c r="G19" s="162" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="105"/>
-      <c r="B20" s="146"/>
-      <c r="C20" s="149"/>
-      <c r="D20" s="143"/>
+      <c r="A20" s="108"/>
+      <c r="B20" s="156"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="153"/>
       <c r="E20" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="151"/>
-      <c r="G20" s="152"/>
+      <c r="F20" s="161"/>
+      <c r="G20" s="162"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="105"/>
-      <c r="B21" s="146"/>
-      <c r="C21" s="149"/>
-      <c r="D21" s="143"/>
+      <c r="A21" s="108"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="153"/>
       <c r="E21" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="151"/>
-      <c r="G21" s="152"/>
+      <c r="F21" s="161"/>
+      <c r="G21" s="162"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="105"/>
-      <c r="B22" s="147"/>
-      <c r="C22" s="150"/>
-      <c r="D22" s="144"/>
+      <c r="A22" s="108"/>
+      <c r="B22" s="157"/>
+      <c r="C22" s="160"/>
+      <c r="D22" s="154"/>
       <c r="E22" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="151"/>
-      <c r="G22" s="152"/>
+      <c r="F22" s="161"/>
+      <c r="G22" s="162"/>
     </row>
     <row r="23" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="105"/>
-      <c r="B23" s="158" t="s">
+      <c r="A23" s="108"/>
+      <c r="B23" s="112" t="s">
         <v>217</v>
       </c>
-      <c r="C23" s="157" t="s">
+      <c r="C23" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="156" t="s">
+      <c r="D23" s="118" t="s">
         <v>52</v>
       </c>
       <c r="E23" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="153" t="s">
+      <c r="F23" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="159" t="s">
+      <c r="G23" s="124" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="105"/>
-      <c r="B24" s="158"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="156"/>
+      <c r="A24" s="108"/>
+      <c r="B24" s="112"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="118"/>
       <c r="E24" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="153"/>
-      <c r="G24" s="159"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="124"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="105"/>
-      <c r="B25" s="158"/>
-      <c r="C25" s="157"/>
-      <c r="D25" s="156"/>
+      <c r="A25" s="108"/>
+      <c r="B25" s="112"/>
+      <c r="C25" s="120"/>
+      <c r="D25" s="118"/>
       <c r="E25" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="153"/>
-      <c r="G25" s="159"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="124"/>
     </row>
     <row r="26" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="105"/>
-      <c r="B26" s="158"/>
-      <c r="C26" s="157"/>
-      <c r="D26" s="156"/>
+      <c r="A26" s="108"/>
+      <c r="B26" s="112"/>
+      <c r="C26" s="120"/>
+      <c r="D26" s="118"/>
       <c r="E26" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="153"/>
-      <c r="G26" s="159"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="124"/>
     </row>
     <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="166"/>
-      <c r="B27" s="162"/>
-      <c r="C27" s="168"/>
-      <c r="D27" s="167"/>
+      <c r="A27" s="117"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="121"/>
+      <c r="D27" s="119"/>
       <c r="E27" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="169"/>
-      <c r="G27" s="170"/>
+      <c r="F27" s="123"/>
+      <c r="G27" s="125"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="172" t="s">
+      <c r="B28" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="C28" s="171" t="s">
+      <c r="C28" s="126" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="126" t="s">
+      <c r="D28" s="165" t="s">
         <v>60</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="173" t="s">
+      <c r="F28" s="132" t="s">
         <v>65</v>
       </c>
-      <c r="G28" s="174" t="s">
+      <c r="G28" s="134" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="105"/>
-      <c r="B29" s="113"/>
-      <c r="C29" s="111"/>
-      <c r="D29" s="125"/>
+      <c r="A29" s="108"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="127"/>
+      <c r="D29" s="130"/>
       <c r="E29" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="107"/>
-      <c r="G29" s="175"/>
+      <c r="F29" s="133"/>
+      <c r="G29" s="135"/>
     </row>
     <row r="30" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="105"/>
-      <c r="B30" s="113"/>
-      <c r="C30" s="111"/>
-      <c r="D30" s="125"/>
+      <c r="A30" s="108"/>
+      <c r="B30" s="129"/>
+      <c r="C30" s="127"/>
+      <c r="D30" s="130"/>
       <c r="E30" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="107"/>
-      <c r="G30" s="175"/>
+      <c r="F30" s="133"/>
+      <c r="G30" s="135"/>
     </row>
     <row r="31" spans="1:17" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="105"/>
-      <c r="B31" s="113"/>
-      <c r="C31" s="111"/>
-      <c r="D31" s="125"/>
+      <c r="A31" s="108"/>
+      <c r="B31" s="129"/>
+      <c r="C31" s="127"/>
+      <c r="D31" s="130"/>
       <c r="E31" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="107"/>
-      <c r="G31" s="176"/>
+      <c r="F31" s="133"/>
+      <c r="G31" s="136"/>
     </row>
     <row r="32" spans="1:17" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="105"/>
+      <c r="A32" s="108"/>
       <c r="B32" s="21" t="s">
         <v>68</v>
       </c>
@@ -3486,7 +3495,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="105"/>
+      <c r="A33" s="108"/>
       <c r="B33" s="21" t="s">
         <v>67</v>
       </c>
@@ -3507,7 +3516,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="105"/>
+      <c r="A34" s="108"/>
       <c r="B34" s="20" t="s">
         <v>78</v>
       </c>
@@ -3517,18 +3526,18 @@
       <c r="D34" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="125" t="s">
+      <c r="E34" s="130" t="s">
         <v>85</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G34" s="109" t="s">
+      <c r="G34" s="131" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="105"/>
+      <c r="A35" s="108"/>
       <c r="B35" s="20" t="s">
         <v>80</v>
       </c>
@@ -3538,68 +3547,68 @@
       <c r="D35" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="125"/>
+      <c r="E35" s="130"/>
       <c r="F35" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G35" s="109"/>
+      <c r="G35" s="131"/>
     </row>
     <row r="36" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="105"/>
-      <c r="B36" s="123" t="s">
+      <c r="A36" s="108"/>
+      <c r="B36" s="169" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="124" t="s">
+      <c r="C36" s="168" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="120" t="s">
+      <c r="D36" s="170" t="s">
         <v>88</v>
       </c>
       <c r="E36" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="121" t="s">
+      <c r="F36" s="166" t="s">
         <v>91</v>
       </c>
-      <c r="G36" s="122" t="s">
+      <c r="G36" s="167" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="105"/>
-      <c r="B37" s="123"/>
-      <c r="C37" s="124"/>
-      <c r="D37" s="120"/>
+      <c r="A37" s="108"/>
+      <c r="B37" s="169"/>
+      <c r="C37" s="168"/>
+      <c r="D37" s="170"/>
       <c r="E37" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="F37" s="121"/>
-      <c r="G37" s="122"/>
+      <c r="F37" s="166"/>
+      <c r="G37" s="167"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="105"/>
-      <c r="B38" s="123"/>
-      <c r="C38" s="124"/>
-      <c r="D38" s="120"/>
+      <c r="A38" s="108"/>
+      <c r="B38" s="169"/>
+      <c r="C38" s="168"/>
+      <c r="D38" s="170"/>
       <c r="E38" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F38" s="121"/>
-      <c r="G38" s="122"/>
+      <c r="F38" s="166"/>
+      <c r="G38" s="167"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="105"/>
-      <c r="B39" s="123"/>
-      <c r="C39" s="124"/>
-      <c r="D39" s="120"/>
+      <c r="A39" s="108"/>
+      <c r="B39" s="169"/>
+      <c r="C39" s="168"/>
+      <c r="D39" s="170"/>
       <c r="E39" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="F39" s="121"/>
-      <c r="G39" s="122"/>
+      <c r="F39" s="166"/>
+      <c r="G39" s="167"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="105"/>
+      <c r="A40" s="108"/>
       <c r="B40" s="20" t="s">
         <v>94</v>
       </c>
@@ -3609,18 +3618,18 @@
       <c r="D40" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="E40" s="125" t="s">
+      <c r="E40" s="130" t="s">
         <v>101</v>
       </c>
-      <c r="F40" s="107" t="s">
+      <c r="F40" s="133" t="s">
         <v>100</v>
       </c>
-      <c r="G40" s="109" t="s">
+      <c r="G40" s="131" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="105"/>
+      <c r="A41" s="108"/>
       <c r="B41" s="20" t="s">
         <v>97</v>
       </c>
@@ -3630,12 +3639,12 @@
       <c r="D41" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="125"/>
-      <c r="F41" s="107"/>
-      <c r="G41" s="109"/>
+      <c r="E41" s="130"/>
+      <c r="F41" s="133"/>
+      <c r="G41" s="131"/>
     </row>
     <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="105"/>
+      <c r="A42" s="108"/>
       <c r="B42" s="21" t="s">
         <v>102</v>
       </c>
@@ -3656,205 +3665,205 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="105"/>
+      <c r="A43" s="108"/>
       <c r="B43" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="111" t="s">
+      <c r="C43" s="127" t="s">
         <v>112</v>
       </c>
-      <c r="D43" s="125" t="s">
+      <c r="D43" s="130" t="s">
         <v>111</v>
       </c>
-      <c r="E43" s="125" t="s">
+      <c r="E43" s="130" t="s">
         <v>113</v>
       </c>
-      <c r="F43" s="107" t="s">
+      <c r="F43" s="133" t="s">
         <v>110</v>
       </c>
-      <c r="G43" s="109" t="s">
+      <c r="G43" s="131" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="105"/>
+      <c r="A44" s="108"/>
       <c r="B44" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="111"/>
-      <c r="D44" s="125"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="107"/>
-      <c r="G44" s="109"/>
+      <c r="C44" s="127"/>
+      <c r="D44" s="130"/>
+      <c r="E44" s="130"/>
+      <c r="F44" s="133"/>
+      <c r="G44" s="131"/>
     </row>
     <row r="45" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="105"/>
-      <c r="B45" s="123" t="s">
+      <c r="A45" s="108"/>
+      <c r="B45" s="169" t="s">
         <v>118</v>
       </c>
-      <c r="C45" s="124" t="s">
+      <c r="C45" s="168" t="s">
         <v>119</v>
       </c>
-      <c r="D45" s="115" t="s">
+      <c r="D45" s="180" t="s">
         <v>128</v>
       </c>
-      <c r="E45" s="120" t="s">
+      <c r="E45" s="170" t="s">
         <v>117</v>
       </c>
-      <c r="F45" s="121" t="s">
+      <c r="F45" s="166" t="s">
         <v>116</v>
       </c>
-      <c r="G45" s="122" t="s">
+      <c r="G45" s="167" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="105"/>
-      <c r="B46" s="123"/>
-      <c r="C46" s="124"/>
-      <c r="D46" s="116"/>
-      <c r="E46" s="120"/>
-      <c r="F46" s="121"/>
-      <c r="G46" s="122"/>
+      <c r="A46" s="108"/>
+      <c r="B46" s="169"/>
+      <c r="C46" s="168"/>
+      <c r="D46" s="181"/>
+      <c r="E46" s="170"/>
+      <c r="F46" s="166"/>
+      <c r="G46" s="167"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="105"/>
-      <c r="B47" s="123"/>
-      <c r="C47" s="124"/>
-      <c r="D47" s="116"/>
-      <c r="E47" s="120"/>
-      <c r="F47" s="121"/>
-      <c r="G47" s="122"/>
+      <c r="A47" s="108"/>
+      <c r="B47" s="169"/>
+      <c r="C47" s="168"/>
+      <c r="D47" s="181"/>
+      <c r="E47" s="170"/>
+      <c r="F47" s="166"/>
+      <c r="G47" s="167"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="105"/>
-      <c r="B48" s="123"/>
-      <c r="C48" s="124"/>
-      <c r="D48" s="116"/>
-      <c r="E48" s="120"/>
-      <c r="F48" s="121"/>
-      <c r="G48" s="122"/>
+      <c r="A48" s="108"/>
+      <c r="B48" s="169"/>
+      <c r="C48" s="168"/>
+      <c r="D48" s="181"/>
+      <c r="E48" s="170"/>
+      <c r="F48" s="166"/>
+      <c r="G48" s="167"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="105"/>
-      <c r="B49" s="123"/>
-      <c r="C49" s="124"/>
-      <c r="D49" s="117"/>
-      <c r="E49" s="120"/>
-      <c r="F49" s="121"/>
-      <c r="G49" s="122"/>
+      <c r="A49" s="108"/>
+      <c r="B49" s="169"/>
+      <c r="C49" s="168"/>
+      <c r="D49" s="182"/>
+      <c r="E49" s="170"/>
+      <c r="F49" s="166"/>
+      <c r="G49" s="167"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="105"/>
-      <c r="B50" s="113" t="s">
+      <c r="A50" s="108"/>
+      <c r="B50" s="129" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="111" t="s">
+      <c r="C50" s="127" t="s">
         <v>122</v>
       </c>
-      <c r="D50" s="118" t="s">
+      <c r="D50" s="183" t="s">
         <v>129</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F50" s="107" t="s">
+      <c r="F50" s="133" t="s">
         <v>127</v>
       </c>
-      <c r="G50" s="109" t="s">
+      <c r="G50" s="131" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="105"/>
-      <c r="B51" s="113"/>
-      <c r="C51" s="111"/>
-      <c r="D51" s="119"/>
+      <c r="A51" s="108"/>
+      <c r="B51" s="129"/>
+      <c r="C51" s="127"/>
+      <c r="D51" s="184"/>
       <c r="E51" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F51" s="107"/>
-      <c r="G51" s="109"/>
+      <c r="F51" s="133"/>
+      <c r="G51" s="131"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="105"/>
-      <c r="B52" s="113"/>
-      <c r="C52" s="111"/>
-      <c r="D52" s="119"/>
+      <c r="A52" s="108"/>
+      <c r="B52" s="129"/>
+      <c r="C52" s="127"/>
+      <c r="D52" s="184"/>
       <c r="E52" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="107"/>
-      <c r="G52" s="109"/>
+      <c r="F52" s="133"/>
+      <c r="G52" s="131"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="105"/>
-      <c r="B53" s="113"/>
-      <c r="C53" s="111"/>
-      <c r="D53" s="119"/>
+      <c r="A53" s="108"/>
+      <c r="B53" s="129"/>
+      <c r="C53" s="127"/>
+      <c r="D53" s="184"/>
       <c r="E53" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="F53" s="107"/>
-      <c r="G53" s="109"/>
+      <c r="F53" s="133"/>
+      <c r="G53" s="131"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="105"/>
-      <c r="B54" s="113"/>
-      <c r="C54" s="111"/>
-      <c r="D54" s="119"/>
+      <c r="A54" s="108"/>
+      <c r="B54" s="129"/>
+      <c r="C54" s="127"/>
+      <c r="D54" s="184"/>
       <c r="E54" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F54" s="107"/>
-      <c r="G54" s="109"/>
+      <c r="F54" s="133"/>
+      <c r="G54" s="131"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="105"/>
-      <c r="B55" s="113"/>
-      <c r="C55" s="111"/>
-      <c r="D55" s="119"/>
+      <c r="A55" s="108"/>
+      <c r="B55" s="129"/>
+      <c r="C55" s="127"/>
+      <c r="D55" s="184"/>
       <c r="E55" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F55" s="107"/>
-      <c r="G55" s="109"/>
+      <c r="F55" s="133"/>
+      <c r="G55" s="131"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="105"/>
-      <c r="B56" s="113"/>
-      <c r="C56" s="111"/>
-      <c r="D56" s="119"/>
+      <c r="A56" s="108"/>
+      <c r="B56" s="129"/>
+      <c r="C56" s="127"/>
+      <c r="D56" s="184"/>
       <c r="E56" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="F56" s="107"/>
-      <c r="G56" s="109"/>
+      <c r="F56" s="133"/>
+      <c r="G56" s="131"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="105"/>
-      <c r="B57" s="113"/>
-      <c r="C57" s="111"/>
-      <c r="D57" s="119"/>
+      <c r="A57" s="108"/>
+      <c r="B57" s="129"/>
+      <c r="C57" s="127"/>
+      <c r="D57" s="184"/>
       <c r="E57" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="F57" s="107"/>
-      <c r="G57" s="109"/>
+      <c r="F57" s="133"/>
+      <c r="G57" s="131"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="106"/>
-      <c r="B58" s="114"/>
-      <c r="C58" s="112"/>
-      <c r="D58" s="119"/>
+      <c r="A58" s="109"/>
+      <c r="B58" s="179"/>
+      <c r="C58" s="178"/>
+      <c r="D58" s="184"/>
       <c r="E58" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F58" s="108"/>
-      <c r="G58" s="110"/>
+      <c r="F58" s="176"/>
+      <c r="G58" s="177"/>
     </row>
     <row r="59" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="104" t="s">
+      <c r="A59" s="107" t="s">
         <v>130</v>
       </c>
       <c r="B59" s="34" t="s">
@@ -3877,7 +3886,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="105"/>
+      <c r="A60" s="108"/>
       <c r="B60" s="43" t="s">
         <v>136</v>
       </c>
@@ -3898,7 +3907,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A61" s="105"/>
+      <c r="A61" s="108"/>
       <c r="B61" s="38" t="s">
         <v>140</v>
       </c>
@@ -3919,7 +3928,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="105"/>
+      <c r="A62" s="108"/>
       <c r="B62" s="43" t="s">
         <v>145</v>
       </c>
@@ -3940,7 +3949,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="105"/>
+      <c r="A63" s="108"/>
       <c r="B63" s="38" t="s">
         <v>149</v>
       </c>
@@ -3961,7 +3970,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="105"/>
+      <c r="A64" s="108"/>
       <c r="B64" s="43" t="s">
         <v>219</v>
       </c>
@@ -3982,7 +3991,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="105"/>
+      <c r="A65" s="108"/>
       <c r="B65" s="38" t="s">
         <v>154</v>
       </c>
@@ -4003,7 +4012,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="105"/>
+      <c r="A66" s="108"/>
       <c r="B66" s="43" t="s">
         <v>155</v>
       </c>
@@ -4024,7 +4033,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="105"/>
+      <c r="A67" s="108"/>
       <c r="B67" s="38" t="s">
         <v>157</v>
       </c>
@@ -4045,7 +4054,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="106"/>
+      <c r="A68" s="109"/>
       <c r="B68" s="59" t="s">
         <v>162</v>
       </c>
@@ -4066,7 +4075,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="104" t="s">
+      <c r="A69" s="107" t="s">
         <v>164</v>
       </c>
       <c r="B69" s="17" t="s">
@@ -4089,7 +4098,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="105"/>
+      <c r="A70" s="108"/>
       <c r="B70" s="19" t="s">
         <v>166</v>
       </c>
@@ -4110,7 +4119,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="105"/>
+      <c r="A71" s="108"/>
       <c r="B71" s="18" t="s">
         <v>167</v>
       </c>
@@ -4131,11 +4140,11 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="105"/>
-      <c r="B72" s="158" t="s">
+      <c r="A72" s="108"/>
+      <c r="B72" s="112" t="s">
         <v>168</v>
       </c>
-      <c r="C72" s="160" t="s">
+      <c r="C72" s="110" t="s">
         <v>186</v>
       </c>
       <c r="D72" s="29" t="s">
@@ -4147,14 +4156,14 @@
       <c r="F72" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="G72" s="163" t="s">
+      <c r="G72" s="114" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="105"/>
-      <c r="B73" s="158"/>
-      <c r="C73" s="160"/>
+      <c r="A73" s="108"/>
+      <c r="B73" s="112"/>
+      <c r="C73" s="110"/>
       <c r="D73" s="29" t="s">
         <v>189</v>
       </c>
@@ -4164,12 +4173,12 @@
       <c r="F73" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="G73" s="164"/>
+      <c r="G73" s="115"/>
     </row>
     <row r="74" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="105"/>
-      <c r="B74" s="158"/>
-      <c r="C74" s="160"/>
+      <c r="A74" s="108"/>
+      <c r="B74" s="112"/>
+      <c r="C74" s="110"/>
       <c r="D74" s="29" t="s">
         <v>190</v>
       </c>
@@ -4179,12 +4188,12 @@
       <c r="F74" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="G74" s="164"/>
+      <c r="G74" s="115"/>
     </row>
     <row r="75" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="105"/>
-      <c r="B75" s="158"/>
-      <c r="C75" s="160"/>
+      <c r="A75" s="108"/>
+      <c r="B75" s="112"/>
+      <c r="C75" s="110"/>
       <c r="D75" s="29" t="s">
         <v>191</v>
       </c>
@@ -4194,12 +4203,12 @@
       <c r="F75" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="G75" s="164"/>
+      <c r="G75" s="115"/>
     </row>
     <row r="76" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="105"/>
-      <c r="B76" s="162"/>
-      <c r="C76" s="161"/>
+      <c r="A76" s="108"/>
+      <c r="B76" s="113"/>
+      <c r="C76" s="111"/>
       <c r="D76" s="57" t="s">
         <v>192</v>
       </c>
@@ -4209,10 +4218,10 @@
       <c r="F76" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="G76" s="165"/>
+      <c r="G76" s="116"/>
     </row>
     <row r="77" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="105"/>
+      <c r="A77" s="108"/>
       <c r="B77" s="69" t="s">
         <v>169</v>
       </c>
@@ -4233,7 +4242,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="105"/>
+      <c r="A78" s="108"/>
       <c r="B78" s="70" t="s">
         <v>170</v>
       </c>
@@ -4254,7 +4263,7 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A79" s="105"/>
+      <c r="A79" s="108"/>
       <c r="B79" s="71" t="s">
         <v>171</v>
       </c>
@@ -4275,7 +4284,7 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A80" s="105"/>
+      <c r="A80" s="108"/>
       <c r="B80" s="70" t="s">
         <v>172</v>
       </c>
@@ -4296,7 +4305,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A81" s="105"/>
+      <c r="A81" s="108"/>
       <c r="B81" s="71" t="s">
         <v>173</v>
       </c>
@@ -4317,7 +4326,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="105"/>
+      <c r="A82" s="108"/>
       <c r="B82" s="70" t="s">
         <v>174</v>
       </c>
@@ -4338,7 +4347,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A83" s="105"/>
+      <c r="A83" s="108"/>
       <c r="B83" s="71" t="s">
         <v>175</v>
       </c>
@@ -4359,7 +4368,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A84" s="105"/>
+      <c r="A84" s="108"/>
       <c r="B84" s="70" t="s">
         <v>176</v>
       </c>
@@ -4380,7 +4389,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A85" s="105"/>
+      <c r="A85" s="108"/>
       <c r="B85" s="71" t="s">
         <v>177</v>
       </c>
@@ -4401,7 +4410,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A86" s="105"/>
+      <c r="A86" s="108"/>
       <c r="B86" s="70" t="s">
         <v>178</v>
       </c>
@@ -4422,7 +4431,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="106"/>
+      <c r="A87" s="109"/>
       <c r="B87" s="75" t="s">
         <v>179</v>
       </c>
@@ -4443,7 +4452,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A88" s="102" t="s">
+      <c r="A88" s="174" t="s">
         <v>261</v>
       </c>
       <c r="B88" s="81" t="s">
@@ -4466,7 +4475,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="103"/>
+      <c r="A89" s="175"/>
       <c r="B89" s="18" t="s">
         <v>263</v>
       </c>
@@ -4487,7 +4496,7 @@
       </c>
     </row>
     <row r="90" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A90" s="103"/>
+      <c r="A90" s="175"/>
       <c r="B90" s="21" t="s">
         <v>264</v>
       </c>
@@ -4508,7 +4517,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A91" s="103"/>
+      <c r="A91" s="175"/>
       <c r="B91" s="18" t="s">
         <v>265</v>
       </c>
@@ -4529,7 +4538,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A92" s="103"/>
+      <c r="A92" s="175"/>
       <c r="B92" s="21" t="s">
         <v>266</v>
       </c>
@@ -4550,7 +4559,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="103"/>
+      <c r="A93" s="175"/>
       <c r="B93" s="18" t="s">
         <v>267</v>
       </c>
@@ -4571,7 +4580,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A94" s="103"/>
+      <c r="A94" s="175"/>
       <c r="B94" s="21" t="s">
         <v>268</v>
       </c>
@@ -4592,7 +4601,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A95" s="103"/>
+      <c r="A95" s="175"/>
       <c r="B95" s="18" t="s">
         <v>269</v>
       </c>
@@ -4613,7 +4622,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A96" s="103"/>
+      <c r="A96" s="175"/>
       <c r="B96" s="21" t="s">
         <v>270</v>
       </c>
@@ -4634,7 +4643,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A97" s="103"/>
+      <c r="A97" s="175"/>
       <c r="B97" s="18" t="s">
         <v>271</v>
       </c>
@@ -4655,7 +4664,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A98" s="103"/>
+      <c r="A98" s="175"/>
       <c r="B98" s="21" t="s">
         <v>272</v>
       </c>
@@ -4676,7 +4685,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A99" s="103"/>
+      <c r="A99" s="175"/>
       <c r="B99" s="18" t="s">
         <v>273</v>
       </c>
@@ -4697,7 +4706,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A100" s="103"/>
+      <c r="A100" s="175"/>
       <c r="B100" s="21" t="s">
         <v>274</v>
       </c>
@@ -4718,7 +4727,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A101" s="103"/>
+      <c r="A101" s="175"/>
       <c r="B101" s="18" t="s">
         <v>275</v>
       </c>
@@ -4739,7 +4748,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A102" s="103"/>
+      <c r="A102" s="175"/>
       <c r="B102" s="21" t="s">
         <v>276</v>
       </c>
@@ -4760,7 +4769,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A103" s="103"/>
+      <c r="A103" s="175"/>
       <c r="B103" s="18" t="s">
         <v>277</v>
       </c>
@@ -4781,7 +4790,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A104" s="103"/>
+      <c r="A104" s="175"/>
       <c r="B104" s="21" t="s">
         <v>278</v>
       </c>
@@ -4802,7 +4811,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A105" s="103"/>
+      <c r="A105" s="175"/>
       <c r="B105" s="18" t="s">
         <v>279</v>
       </c>
@@ -4823,7 +4832,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A106" s="103"/>
+      <c r="A106" s="175"/>
       <c r="B106" s="21" t="s">
         <v>280</v>
       </c>
@@ -4844,7 +4853,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A107" s="103"/>
+      <c r="A107" s="175"/>
       <c r="B107" s="18" t="s">
         <v>281</v>
       </c>
@@ -4865,7 +4874,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="103"/>
+      <c r="A108" s="175"/>
       <c r="B108" s="91" t="s">
         <v>282</v>
       </c>
@@ -4886,7 +4895,7 @@
       </c>
     </row>
     <row r="109" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A109" s="100" t="s">
+      <c r="A109" s="171" t="s">
         <v>374</v>
       </c>
       <c r="B109" s="17" t="s">
@@ -4909,7 +4918,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="101"/>
+      <c r="A110" s="172"/>
       <c r="B110" s="80" t="s">
         <v>376</v>
       </c>
@@ -4930,7 +4939,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A111" s="101"/>
+      <c r="A111" s="172"/>
       <c r="B111" s="18" t="s">
         <v>377</v>
       </c>
@@ -4951,7 +4960,7 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="173.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="101"/>
+      <c r="A112" s="172"/>
       <c r="B112" s="19" t="s">
         <v>378</v>
       </c>
@@ -4972,7 +4981,7 @@
       </c>
     </row>
     <row r="113" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="101"/>
+      <c r="A113" s="172"/>
       <c r="B113" s="18" t="s">
         <v>379</v>
       </c>
@@ -4993,7 +5002,7 @@
       </c>
     </row>
     <row r="114" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A114" s="101"/>
+      <c r="A114" s="172"/>
       <c r="B114" s="19" t="s">
         <v>380</v>
       </c>
@@ -5014,11 +5023,11 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="173.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="177"/>
+      <c r="A115" s="173"/>
       <c r="B115" s="90" t="s">
         <v>381</v>
       </c>
-      <c r="C115" s="178" t="s">
+      <c r="C115" s="100" t="s">
         <v>409</v>
       </c>
       <c r="D115" s="77" t="s">
@@ -5035,186 +5044,203 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A116" s="179" t="s">
+      <c r="A116" s="104" t="s">
         <v>415</v>
       </c>
-      <c r="B116" s="183" t="s">
+      <c r="B116" s="102" t="s">
         <v>416</v>
       </c>
       <c r="C116" s="82" t="s">
+        <v>424</v>
+      </c>
+      <c r="D116" s="83" t="s">
+        <v>427</v>
+      </c>
+      <c r="E116" s="83" t="s">
+        <v>428</v>
+      </c>
+      <c r="F116" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="G116" s="85" t="s">
         <v>425</v>
       </c>
-      <c r="D116" s="83" t="s">
-        <v>428</v>
-      </c>
-      <c r="E116" s="83" t="s">
-        <v>429</v>
-      </c>
-      <c r="F116" s="84" t="s">
-        <v>427</v>
-      </c>
-      <c r="G116" s="85" t="s">
-        <v>426</v>
-      </c>
     </row>
     <row r="117" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A117" s="180"/>
+      <c r="A117" s="105"/>
       <c r="B117" s="38" t="s">
         <v>417</v>
       </c>
       <c r="C117" s="42" t="s">
+        <v>429</v>
+      </c>
+      <c r="D117" s="40" t="s">
+        <v>432</v>
+      </c>
+      <c r="E117" s="40" t="s">
+        <v>440</v>
+      </c>
+      <c r="F117" s="41" t="s">
         <v>430</v>
       </c>
-      <c r="D117" s="40" t="s">
+      <c r="G117" s="53" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A118" s="105"/>
+      <c r="B118" s="103" t="s">
+        <v>418</v>
+      </c>
+      <c r="C118" s="86" t="s">
+        <v>424</v>
+      </c>
+      <c r="D118" s="87" t="s">
+        <v>434</v>
+      </c>
+      <c r="E118" s="87" t="s">
+        <v>435</v>
+      </c>
+      <c r="F118" s="88" t="s">
+        <v>438</v>
+      </c>
+      <c r="G118" s="89" t="s">
         <v>433</v>
       </c>
-      <c r="E117" s="40" t="s">
-        <v>441</v>
-      </c>
-      <c r="F117" s="41" t="s">
-        <v>431</v>
-      </c>
-      <c r="G117" s="53" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A118" s="180"/>
-      <c r="B118" s="184" t="s">
-        <v>418</v>
-      </c>
-      <c r="C118" s="86" t="s">
-        <v>425</v>
-      </c>
-      <c r="D118" s="87" t="s">
-        <v>435</v>
-      </c>
-      <c r="E118" s="87" t="s">
-        <v>436</v>
-      </c>
-      <c r="F118" s="88" t="s">
-        <v>439</v>
-      </c>
-      <c r="G118" s="89" t="s">
-        <v>434</v>
-      </c>
     </row>
     <row r="119" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="180"/>
+      <c r="A119" s="105"/>
       <c r="B119" s="38" t="s">
         <v>419</v>
       </c>
       <c r="C119" s="42" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D119" s="40" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E119" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="F119" s="41" t="s">
+        <v>437</v>
+      </c>
+      <c r="G119" s="53" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A120" s="105"/>
+      <c r="B120" s="103" t="s">
+        <v>420</v>
+      </c>
+      <c r="C120" s="86" t="s">
         <v>442</v>
       </c>
-      <c r="F119" s="41" t="s">
-        <v>438</v>
-      </c>
-      <c r="G119" s="53" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A120" s="180"/>
-      <c r="B120" s="184" t="s">
-        <v>420</v>
-      </c>
-      <c r="C120" s="86" t="s">
+      <c r="D120" s="87" t="s">
+        <v>445</v>
+      </c>
+      <c r="E120" s="87" t="s">
+        <v>444</v>
+      </c>
+      <c r="F120" s="88" t="s">
+        <v>446</v>
+      </c>
+      <c r="G120" s="89" t="s">
         <v>443</v>
       </c>
-      <c r="D120" s="87" t="s">
-        <v>446</v>
-      </c>
-      <c r="E120" s="87" t="s">
-        <v>445</v>
-      </c>
-      <c r="F120" s="88" t="s">
-        <v>447</v>
-      </c>
-      <c r="G120" s="89" t="s">
-        <v>444</v>
-      </c>
     </row>
     <row r="121" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A121" s="180"/>
+      <c r="A121" s="105"/>
       <c r="B121" s="38" t="s">
         <v>421</v>
       </c>
       <c r="C121" s="42" t="s">
+        <v>448</v>
+      </c>
+      <c r="D121" s="40" t="s">
         <v>449</v>
       </c>
-      <c r="D121" s="40" t="s">
+      <c r="E121" s="40" t="s">
         <v>450</v>
       </c>
-      <c r="E121" s="40" t="s">
+      <c r="F121" s="41" t="s">
         <v>451</v>
       </c>
-      <c r="F121" s="41" t="s">
+      <c r="G121" s="53" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="A122" s="105"/>
+      <c r="B122" s="103" t="s">
+        <v>422</v>
+      </c>
+      <c r="C122" s="86" t="s">
         <v>452</v>
       </c>
-      <c r="G121" s="53" t="s">
+      <c r="D122" s="87" t="s">
+        <v>455</v>
+      </c>
+      <c r="E122" s="87" t="s">
+        <v>454</v>
+      </c>
+      <c r="F122" s="88" t="s">
+        <v>456</v>
+      </c>
+      <c r="G122" s="89" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="106"/>
+      <c r="B123" s="101" t="s">
+        <v>423</v>
+      </c>
+      <c r="C123" s="96" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A122" s="180"/>
-      <c r="B122" s="184" t="s">
-        <v>422</v>
-      </c>
-      <c r="C122" s="86" t="s">
-        <v>453</v>
-      </c>
-      <c r="D122" s="87" t="s">
-        <v>456</v>
-      </c>
-      <c r="E122" s="87" t="s">
-        <v>455</v>
-      </c>
-      <c r="F122" s="88" t="s">
+      <c r="D123" s="97" t="s">
+        <v>459</v>
+      </c>
+      <c r="E123" s="97" t="s">
+        <v>450</v>
+      </c>
+      <c r="F123" s="98" t="s">
         <v>457</v>
       </c>
-      <c r="G122" s="89" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="181"/>
-      <c r="B123" s="182" t="s">
-        <v>423</v>
-      </c>
-      <c r="C123" s="96"/>
-      <c r="D123" s="97"/>
-      <c r="E123" s="97"/>
-      <c r="F123" s="98" t="s">
-        <v>424</v>
-      </c>
-      <c r="G123" s="98"/>
+      <c r="G123" s="185" t="s">
+        <v>458</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="A116:A123"/>
-    <mergeCell ref="A69:A87"/>
-    <mergeCell ref="C72:C76"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="G72:G76"/>
-    <mergeCell ref="A4:A27"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="G23:G27"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="A59:A68"/>
+    <mergeCell ref="F50:F58"/>
+    <mergeCell ref="G50:G58"/>
+    <mergeCell ref="C50:C58"/>
+    <mergeCell ref="B50:B58"/>
+    <mergeCell ref="A28:A58"/>
+    <mergeCell ref="D45:D49"/>
+    <mergeCell ref="D50:D58"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="F45:F49"/>
+    <mergeCell ref="G45:G49"/>
+    <mergeCell ref="B45:B49"/>
+    <mergeCell ref="C45:C49"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="G36:G39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="D36:D39"/>
     <mergeCell ref="A1:G2"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
@@ -5231,35 +5257,26 @@
     <mergeCell ref="B11:B18"/>
     <mergeCell ref="F11:F18"/>
     <mergeCell ref="G11:G18"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="G28:G31"/>
     <mergeCell ref="D28:D31"/>
-    <mergeCell ref="F36:F39"/>
-    <mergeCell ref="G36:G39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="A4:A27"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="A116:A123"/>
+    <mergeCell ref="A69:A87"/>
+    <mergeCell ref="C72:C76"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="G72:G76"/>
     <mergeCell ref="A109:A115"/>
     <mergeCell ref="A88:A108"/>
-    <mergeCell ref="A59:A68"/>
-    <mergeCell ref="F50:F58"/>
-    <mergeCell ref="G50:G58"/>
-    <mergeCell ref="C50:C58"/>
-    <mergeCell ref="B50:B58"/>
-    <mergeCell ref="A28:A58"/>
-    <mergeCell ref="D45:D49"/>
-    <mergeCell ref="D50:D58"/>
-    <mergeCell ref="E45:E49"/>
-    <mergeCell ref="F45:F49"/>
-    <mergeCell ref="G45:G49"/>
-    <mergeCell ref="B45:B49"/>
-    <mergeCell ref="C45:C49"/>
-    <mergeCell ref="F43:F44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G9" r:id="rId1" location="L7" xr:uid="{F521EE9C-24C9-46E9-9B83-619AF2EE0F94}"/>
@@ -5337,8 +5354,9 @@
     <hyperlink ref="G120" r:id="rId73" location="L51" xr:uid="{8ECF7719-5670-4B3F-B9C3-C3197DFD337B}"/>
     <hyperlink ref="G121" r:id="rId74" location="L109" xr:uid="{FED95FC2-CDCC-44EC-BD1B-436544254C59}"/>
     <hyperlink ref="G122" r:id="rId75" location="L66" xr:uid="{138045F9-41E1-4E3B-B191-777BEB42D922}"/>
+    <hyperlink ref="G123" r:id="rId76" location="L60" xr:uid="{59C06E23-9121-4645-8FD0-31CC6C9006A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId76"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId77"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the absent function
</commit_message>
<xml_diff>
--- a/EIS_TOOL.xlsx
+++ b/EIS_TOOL.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BEAK_Arbeit\EIS_TOOLKIT_FUNCTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB22D8B-441A-430D-A7A2-C8513B317F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E947A3-9ADE-48A4-9D25-F69C633A3F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C5D5763F-541F-4E53-AD9E-96294ACC5C82}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TOOLKIT Funktionen" sheetId="1" r:id="rId1"/>
+    <sheet name="Fehlende Funktionen" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="499">
   <si>
     <t>EIS_TOOLKIT</t>
   </si>
@@ -1603,6 +1604,125 @@
   </si>
   <si>
     <t xml:space="preserve">single_plr_transform, _single_plr_transform,  _single_plr_transform_by_index, _calculate_plr_scaling_factor, </t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Check raster grids</t>
+  </si>
+  <si>
+    <t>Combine raster bands</t>
+  </si>
+  <si>
+    <t>Convert raster nodata</t>
+  </si>
+  <si>
+    <t>Replace with nodata</t>
+  </si>
+  <si>
+    <t>Unify raster nodata</t>
+  </si>
+  <si>
+    <t>Set raster nodata</t>
+  </si>
+  <si>
+    <t>Split raster bands</t>
+  </si>
+  <si>
+    <t>Check if raster grids have same CRS, alignment, pixel size and optionally extent.</t>
+  </si>
+  <si>
+    <t>Combine multiple rasters into one multiband raster.</t>
+  </si>
+  <si>
+    <t>plot_prediction_area_curves.py</t>
+  </si>
+  <si>
+    <t>evaluation_functions.ipynb (Jupyternotebook)</t>
+  </si>
+  <si>
+    <t>Link wo das Funktion aufgerufen wird</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/46cc25c1de69ee8b66c7a752ba5dfa47d33847c1/notebooks/evaluation_functions.ipynb#L28</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/master/eis_toolkit/evaluation/plot_prediction_area_curves.py#L58</t>
+  </si>
+  <si>
+    <t>aufgerufen</t>
+  </si>
+  <si>
+    <t>calculate_base_metrics.py</t>
+  </si>
+  <si>
+    <t>algorithms/drafts/calculate_base_metrics.py, plot_prediction_area_curves (Nicht direkt aufgerufen im plot_prediction_area_curves, es dient als Eingabeschöpfer für die gegebene Funktion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate_base_metrics, _calculate_base_metrics, </t>
+  </si>
+  <si>
+    <t>geopandas, numpy, pandas, rasterio, eis_toolkit.utilities.checks.geometry -&gt; check_geometry_types,  eis_toolkit.utilities.checks.raster -&gt; check_matching_crs</t>
+  </si>
+  <si>
+    <t>Berechne Werte für die wahre positive Rate, den Anteil der Fläche und die falsche positive Rate für verschiedene Schwellenwerte.
+Die Funktion berechnet die wahre positive Rate, den Anteil der Fläche und die falsche positive Rate für verschiedene Schwellenwerte, die anhand der eingegebenen Ablagerungsorte und der Mineralprospektivitätskarte bestimmt werden. Beachte, dass die Berechnung der falschen positiven Rate optional ist und nur durchgeführt wird, wenn negative Punktorte angegeben werden.</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/master/eis_toolkit/evaluation/calculate_base_metrics.py</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_qgis_plugin/blob/535bcbc77bf937aa6ac70d2a112efb884e290b20/eis_qgis_plugin/eis_processing/algorithms/drafts/calculate_base_metrics.py#L4</t>
+  </si>
+  <si>
+    <t>plot_nn_model_performance.py</t>
+  </si>
+  <si>
+    <t>plot_nn_model_accuracy, plot_nn_model_loss</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>matplotlib.pyplot, pandas, seaborn, eis_toolkit.exceptions -&gt; InvalidDatasetException, InvalidDataShapeException</t>
+  </si>
+  <si>
+    <t>Plotte Trainings- und Validierungsgenauigkeiten für ein neuronales Netzwerkmodell.
+Plotte Trainings- und Validierungsverluste für ein neuronales Netzwerkmodell.</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/master/eis_toolkit/evaluation/plot_nn_model_performance.py</t>
+  </si>
+  <si>
+    <t>matplotlib, numpy, pandas, matplotlib -&gt;  pyplot, shapely.geometry -&gt; LineString, eis_toolkit.exceptions -&gt; InvalidParameterValueException</t>
+  </si>
+  <si>
+    <t>plot_prediction_area_curves, _plot_prediction_area_curves, _get_pa_intersection</t>
+  </si>
+  <si>
+    <t>Plotte das Vorhersage-Flächen (P-A) Diagramm.</t>
+  </si>
+  <si>
+    <t>plot_rate_curve.py</t>
+  </si>
+  <si>
+    <t>plot_rate_curve, _plot_rate_curve</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/master/eis_toolkit/evaluation/plot_rate_curve.py</t>
+  </si>
+  <si>
+    <t>evaluation_functions.ipynb</t>
+  </si>
+  <si>
+    <t>https://github.com/GispoCoding/eis_toolkit/blob/46cc25c1de69ee8b66c7a752ba5dfa47d33847c1/notebooks/evaluation_functions.ipynb#L27</t>
+  </si>
+  <si>
+    <t>matplotlib, numpy, pandas, matplotlib -&gt; pyplot, sklearn.metrics -&gt; auc, eis_toolkit.exceptions -&gt; InvalidParameterValueException</t>
+  </si>
+  <si>
+    <t>Plotte die Erfolgsrate</t>
   </si>
 </sst>
 </file>
@@ -1671,7 +1791,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1702,6 +1822,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -2036,7 +2168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -2319,39 +2451,27 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2382,6 +2502,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2442,6 +2571,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2526,9 +2658,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2544,21 +2673,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2586,8 +2700,111 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2929,12 +3146,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A14118C-3B2E-47A8-AB52-8BB0F98EF7A4}">
-  <dimension ref="A1:Q123"/>
+  <dimension ref="A1:Q130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A116" sqref="A116:A123"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2992,7 +3209,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="103" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -3015,7 +3232,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="108"/>
+      <c r="A5" s="104"/>
       <c r="B5" s="143" t="s">
         <v>213</v>
       </c>
@@ -3028,7 +3245,7 @@
       <c r="E5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="122" t="s">
+      <c r="F5" s="121" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="163" t="s">
@@ -3036,29 +3253,29 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="108"/>
+      <c r="A6" s="104"/>
       <c r="B6" s="144"/>
       <c r="C6" s="147"/>
       <c r="D6" s="150"/>
       <c r="E6" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="122"/>
+      <c r="F6" s="121"/>
       <c r="G6" s="164"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="108"/>
+      <c r="A7" s="104"/>
       <c r="B7" s="145"/>
       <c r="C7" s="148"/>
       <c r="D7" s="151"/>
       <c r="E7" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="122"/>
+      <c r="F7" s="121"/>
       <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="108"/>
+      <c r="A8" s="104"/>
       <c r="B8" s="18" t="s">
         <v>21</v>
       </c>
@@ -3079,7 +3296,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="108"/>
+      <c r="A9" s="104"/>
       <c r="B9" s="19" t="s">
         <v>214</v>
       </c>
@@ -3100,7 +3317,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="108"/>
+      <c r="A10" s="104"/>
       <c r="B10" s="18" t="s">
         <v>215</v>
       </c>
@@ -3121,23 +3338,23 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="108"/>
-      <c r="B11" s="112" t="s">
+      <c r="A11" s="104"/>
+      <c r="B11" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="119" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="118" t="s">
+      <c r="D11" s="117" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="122" t="s">
+      <c r="F11" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="124" t="s">
+      <c r="G11" s="123" t="s">
         <v>45</v>
       </c>
       <c r="H11" s="2"/>
@@ -3152,15 +3369,15 @@
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="108"/>
-      <c r="B12" s="112"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="118"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="117"/>
       <c r="E12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="122"/>
-      <c r="G12" s="124"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="123"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -3173,15 +3390,15 @@
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="108"/>
-      <c r="B13" s="112"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="118"/>
+      <c r="A13" s="104"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="117"/>
       <c r="E13" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="122"/>
-      <c r="G13" s="124"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="123"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -3194,15 +3411,15 @@
       <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="108"/>
-      <c r="B14" s="112"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="118"/>
+      <c r="A14" s="104"/>
+      <c r="B14" s="108"/>
+      <c r="C14" s="119"/>
+      <c r="D14" s="117"/>
       <c r="E14" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="122"/>
-      <c r="G14" s="124"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="123"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -3215,15 +3432,15 @@
       <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="108"/>
-      <c r="B15" s="112"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="118"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="117"/>
       <c r="E15" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="122"/>
-      <c r="G15" s="124"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="123"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -3236,15 +3453,15 @@
       <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="108"/>
-      <c r="B16" s="112"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="118"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="117"/>
       <c r="E16" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="122"/>
-      <c r="G16" s="124"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="123"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -3257,15 +3474,15 @@
       <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="108"/>
-      <c r="B17" s="112"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="118"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="117"/>
       <c r="E17" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="122"/>
-      <c r="G17" s="124"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="123"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -3278,15 +3495,15 @@
       <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="108"/>
-      <c r="B18" s="112"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="118"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="108"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="117"/>
       <c r="E18" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="122"/>
-      <c r="G18" s="124"/>
+      <c r="F18" s="121"/>
+      <c r="G18" s="123"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -3299,7 +3516,7 @@
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="108"/>
+      <c r="A19" s="104"/>
       <c r="B19" s="155" t="s">
         <v>216</v>
       </c>
@@ -3320,7 +3537,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="108"/>
+      <c r="A20" s="104"/>
       <c r="B20" s="156"/>
       <c r="C20" s="159"/>
       <c r="D20" s="153"/>
@@ -3331,7 +3548,7 @@
       <c r="G20" s="162"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="108"/>
+      <c r="A21" s="104"/>
       <c r="B21" s="156"/>
       <c r="C21" s="159"/>
       <c r="D21" s="153"/>
@@ -3342,7 +3559,7 @@
       <c r="G21" s="162"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="108"/>
+      <c r="A22" s="104"/>
       <c r="B22" s="157"/>
       <c r="C22" s="160"/>
       <c r="D22" s="154"/>
@@ -3353,128 +3570,128 @@
       <c r="G22" s="162"/>
     </row>
     <row r="23" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="108"/>
-      <c r="B23" s="112" t="s">
+      <c r="A23" s="104"/>
+      <c r="B23" s="108" t="s">
         <v>217</v>
       </c>
-      <c r="C23" s="120" t="s">
+      <c r="C23" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="118" t="s">
+      <c r="D23" s="117" t="s">
         <v>52</v>
       </c>
       <c r="E23" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="122" t="s">
+      <c r="F23" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="124" t="s">
+      <c r="G23" s="123" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="108"/>
-      <c r="B24" s="112"/>
-      <c r="C24" s="120"/>
-      <c r="D24" s="118"/>
+      <c r="A24" s="104"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="117"/>
       <c r="E24" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="122"/>
-      <c r="G24" s="124"/>
+      <c r="F24" s="121"/>
+      <c r="G24" s="123"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="108"/>
-      <c r="B25" s="112"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="118"/>
+      <c r="A25" s="104"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="117"/>
       <c r="E25" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="122"/>
-      <c r="G25" s="124"/>
+      <c r="F25" s="121"/>
+      <c r="G25" s="123"/>
     </row>
     <row r="26" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="108"/>
-      <c r="B26" s="112"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="118"/>
+      <c r="A26" s="104"/>
+      <c r="B26" s="108"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="117"/>
       <c r="E26" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="122"/>
-      <c r="G26" s="124"/>
+      <c r="F26" s="121"/>
+      <c r="G26" s="123"/>
     </row>
     <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="117"/>
-      <c r="B27" s="113"/>
-      <c r="C27" s="121"/>
-      <c r="D27" s="119"/>
+      <c r="A27" s="116"/>
+      <c r="B27" s="109"/>
+      <c r="C27" s="120"/>
+      <c r="D27" s="118"/>
       <c r="E27" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="123"/>
-      <c r="G27" s="125"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="124"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="107" t="s">
+      <c r="A28" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="128" t="s">
+      <c r="B28" s="127" t="s">
         <v>218</v>
       </c>
-      <c r="C28" s="126" t="s">
+      <c r="C28" s="125" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="165" t="s">
+      <c r="D28" s="136" t="s">
         <v>60</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="132" t="s">
+      <c r="F28" s="131" t="s">
         <v>65</v>
       </c>
-      <c r="G28" s="134" t="s">
+      <c r="G28" s="133" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="108"/>
-      <c r="B29" s="129"/>
-      <c r="C29" s="127"/>
-      <c r="D29" s="130"/>
+      <c r="A29" s="104"/>
+      <c r="B29" s="128"/>
+      <c r="C29" s="126"/>
+      <c r="D29" s="129"/>
       <c r="E29" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="133"/>
-      <c r="G29" s="135"/>
+      <c r="F29" s="132"/>
+      <c r="G29" s="134"/>
     </row>
     <row r="30" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="108"/>
-      <c r="B30" s="129"/>
-      <c r="C30" s="127"/>
-      <c r="D30" s="130"/>
+      <c r="A30" s="104"/>
+      <c r="B30" s="128"/>
+      <c r="C30" s="126"/>
+      <c r="D30" s="129"/>
       <c r="E30" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="133"/>
-      <c r="G30" s="135"/>
+      <c r="F30" s="132"/>
+      <c r="G30" s="134"/>
     </row>
     <row r="31" spans="1:17" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="108"/>
-      <c r="B31" s="129"/>
-      <c r="C31" s="127"/>
-      <c r="D31" s="130"/>
+      <c r="A31" s="104"/>
+      <c r="B31" s="128"/>
+      <c r="C31" s="126"/>
+      <c r="D31" s="129"/>
       <c r="E31" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="133"/>
-      <c r="G31" s="136"/>
+      <c r="F31" s="132"/>
+      <c r="G31" s="135"/>
     </row>
     <row r="32" spans="1:17" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="108"/>
+      <c r="A32" s="104"/>
       <c r="B32" s="21" t="s">
         <v>68</v>
       </c>
@@ -3495,7 +3712,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="108"/>
+      <c r="A33" s="104"/>
       <c r="B33" s="21" t="s">
         <v>67</v>
       </c>
@@ -3516,7 +3733,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="108"/>
+      <c r="A34" s="104"/>
       <c r="B34" s="20" t="s">
         <v>78</v>
       </c>
@@ -3526,18 +3743,18 @@
       <c r="D34" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="130" t="s">
+      <c r="E34" s="129" t="s">
         <v>85</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G34" s="131" t="s">
+      <c r="G34" s="130" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="108"/>
+      <c r="A35" s="104"/>
       <c r="B35" s="20" t="s">
         <v>80</v>
       </c>
@@ -3547,68 +3764,68 @@
       <c r="D35" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="130"/>
+      <c r="E35" s="129"/>
       <c r="F35" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G35" s="131"/>
+      <c r="G35" s="130"/>
     </row>
     <row r="36" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="108"/>
-      <c r="B36" s="169" t="s">
+      <c r="A36" s="104"/>
+      <c r="B36" s="168" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="168" t="s">
+      <c r="C36" s="167" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="170" t="s">
+      <c r="D36" s="169" t="s">
         <v>88</v>
       </c>
       <c r="E36" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="166" t="s">
+      <c r="F36" s="165" t="s">
         <v>91</v>
       </c>
-      <c r="G36" s="167" t="s">
+      <c r="G36" s="166" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="108"/>
-      <c r="B37" s="169"/>
-      <c r="C37" s="168"/>
-      <c r="D37" s="170"/>
+      <c r="A37" s="104"/>
+      <c r="B37" s="168"/>
+      <c r="C37" s="167"/>
+      <c r="D37" s="169"/>
       <c r="E37" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="F37" s="166"/>
-      <c r="G37" s="167"/>
+      <c r="F37" s="165"/>
+      <c r="G37" s="166"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="108"/>
-      <c r="B38" s="169"/>
-      <c r="C38" s="168"/>
-      <c r="D38" s="170"/>
+      <c r="A38" s="104"/>
+      <c r="B38" s="168"/>
+      <c r="C38" s="167"/>
+      <c r="D38" s="169"/>
       <c r="E38" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F38" s="166"/>
-      <c r="G38" s="167"/>
+      <c r="F38" s="165"/>
+      <c r="G38" s="166"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="108"/>
-      <c r="B39" s="169"/>
-      <c r="C39" s="168"/>
-      <c r="D39" s="170"/>
+      <c r="A39" s="104"/>
+      <c r="B39" s="168"/>
+      <c r="C39" s="167"/>
+      <c r="D39" s="169"/>
       <c r="E39" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="F39" s="166"/>
-      <c r="G39" s="167"/>
+      <c r="F39" s="165"/>
+      <c r="G39" s="166"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="108"/>
+      <c r="A40" s="104"/>
       <c r="B40" s="20" t="s">
         <v>94</v>
       </c>
@@ -3618,18 +3835,18 @@
       <c r="D40" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="E40" s="130" t="s">
+      <c r="E40" s="129" t="s">
         <v>101</v>
       </c>
-      <c r="F40" s="133" t="s">
+      <c r="F40" s="132" t="s">
         <v>100</v>
       </c>
-      <c r="G40" s="131" t="s">
+      <c r="G40" s="130" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="108"/>
+      <c r="A41" s="104"/>
       <c r="B41" s="20" t="s">
         <v>97</v>
       </c>
@@ -3639,12 +3856,12 @@
       <c r="D41" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="130"/>
-      <c r="F41" s="133"/>
-      <c r="G41" s="131"/>
+      <c r="E41" s="129"/>
+      <c r="F41" s="132"/>
+      <c r="G41" s="130"/>
     </row>
     <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="108"/>
+      <c r="A42" s="104"/>
       <c r="B42" s="21" t="s">
         <v>102</v>
       </c>
@@ -3665,205 +3882,205 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="108"/>
+      <c r="A43" s="104"/>
       <c r="B43" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="127" t="s">
+      <c r="C43" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="D43" s="130" t="s">
+      <c r="D43" s="129" t="s">
         <v>111</v>
       </c>
-      <c r="E43" s="130" t="s">
+      <c r="E43" s="129" t="s">
         <v>113</v>
       </c>
-      <c r="F43" s="133" t="s">
+      <c r="F43" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="G43" s="131" t="s">
+      <c r="G43" s="130" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="108"/>
+      <c r="A44" s="104"/>
       <c r="B44" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="127"/>
-      <c r="D44" s="130"/>
-      <c r="E44" s="130"/>
-      <c r="F44" s="133"/>
-      <c r="G44" s="131"/>
+      <c r="C44" s="126"/>
+      <c r="D44" s="129"/>
+      <c r="E44" s="129"/>
+      <c r="F44" s="132"/>
+      <c r="G44" s="130"/>
     </row>
     <row r="45" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="108"/>
-      <c r="B45" s="169" t="s">
+      <c r="A45" s="104"/>
+      <c r="B45" s="168" t="s">
         <v>118</v>
       </c>
-      <c r="C45" s="168" t="s">
+      <c r="C45" s="167" t="s">
         <v>119</v>
       </c>
-      <c r="D45" s="180" t="s">
+      <c r="D45" s="174" t="s">
         <v>128</v>
       </c>
-      <c r="E45" s="170" t="s">
+      <c r="E45" s="169" t="s">
         <v>117</v>
       </c>
-      <c r="F45" s="166" t="s">
+      <c r="F45" s="165" t="s">
         <v>116</v>
       </c>
-      <c r="G45" s="167" t="s">
+      <c r="G45" s="166" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="108"/>
-      <c r="B46" s="169"/>
-      <c r="C46" s="168"/>
-      <c r="D46" s="181"/>
-      <c r="E46" s="170"/>
-      <c r="F46" s="166"/>
-      <c r="G46" s="167"/>
+      <c r="A46" s="104"/>
+      <c r="B46" s="168"/>
+      <c r="C46" s="167"/>
+      <c r="D46" s="175"/>
+      <c r="E46" s="169"/>
+      <c r="F46" s="165"/>
+      <c r="G46" s="166"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="108"/>
-      <c r="B47" s="169"/>
-      <c r="C47" s="168"/>
-      <c r="D47" s="181"/>
-      <c r="E47" s="170"/>
-      <c r="F47" s="166"/>
-      <c r="G47" s="167"/>
+      <c r="A47" s="104"/>
+      <c r="B47" s="168"/>
+      <c r="C47" s="167"/>
+      <c r="D47" s="175"/>
+      <c r="E47" s="169"/>
+      <c r="F47" s="165"/>
+      <c r="G47" s="166"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="108"/>
-      <c r="B48" s="169"/>
-      <c r="C48" s="168"/>
-      <c r="D48" s="181"/>
-      <c r="E48" s="170"/>
-      <c r="F48" s="166"/>
-      <c r="G48" s="167"/>
+      <c r="A48" s="104"/>
+      <c r="B48" s="168"/>
+      <c r="C48" s="167"/>
+      <c r="D48" s="175"/>
+      <c r="E48" s="169"/>
+      <c r="F48" s="165"/>
+      <c r="G48" s="166"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="108"/>
-      <c r="B49" s="169"/>
-      <c r="C49" s="168"/>
-      <c r="D49" s="182"/>
-      <c r="E49" s="170"/>
-      <c r="F49" s="166"/>
-      <c r="G49" s="167"/>
+      <c r="A49" s="104"/>
+      <c r="B49" s="168"/>
+      <c r="C49" s="167"/>
+      <c r="D49" s="176"/>
+      <c r="E49" s="169"/>
+      <c r="F49" s="165"/>
+      <c r="G49" s="166"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="108"/>
-      <c r="B50" s="129" t="s">
+      <c r="A50" s="104"/>
+      <c r="B50" s="128" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="127" t="s">
+      <c r="C50" s="126" t="s">
         <v>122</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="177" t="s">
         <v>129</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F50" s="133" t="s">
+      <c r="F50" s="132" t="s">
         <v>127</v>
       </c>
-      <c r="G50" s="131" t="s">
+      <c r="G50" s="130" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="108"/>
-      <c r="B51" s="129"/>
-      <c r="C51" s="127"/>
-      <c r="D51" s="184"/>
+      <c r="A51" s="104"/>
+      <c r="B51" s="128"/>
+      <c r="C51" s="126"/>
+      <c r="D51" s="178"/>
       <c r="E51" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F51" s="133"/>
-      <c r="G51" s="131"/>
+      <c r="F51" s="132"/>
+      <c r="G51" s="130"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="108"/>
-      <c r="B52" s="129"/>
-      <c r="C52" s="127"/>
-      <c r="D52" s="184"/>
+      <c r="A52" s="104"/>
+      <c r="B52" s="128"/>
+      <c r="C52" s="126"/>
+      <c r="D52" s="178"/>
       <c r="E52" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="133"/>
-      <c r="G52" s="131"/>
+      <c r="F52" s="132"/>
+      <c r="G52" s="130"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="108"/>
-      <c r="B53" s="129"/>
-      <c r="C53" s="127"/>
-      <c r="D53" s="184"/>
+      <c r="A53" s="104"/>
+      <c r="B53" s="128"/>
+      <c r="C53" s="126"/>
+      <c r="D53" s="178"/>
       <c r="E53" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="F53" s="133"/>
-      <c r="G53" s="131"/>
+      <c r="F53" s="132"/>
+      <c r="G53" s="130"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="108"/>
-      <c r="B54" s="129"/>
-      <c r="C54" s="127"/>
-      <c r="D54" s="184"/>
+      <c r="A54" s="104"/>
+      <c r="B54" s="128"/>
+      <c r="C54" s="126"/>
+      <c r="D54" s="178"/>
       <c r="E54" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F54" s="133"/>
-      <c r="G54" s="131"/>
+      <c r="F54" s="132"/>
+      <c r="G54" s="130"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="108"/>
-      <c r="B55" s="129"/>
-      <c r="C55" s="127"/>
-      <c r="D55" s="184"/>
+      <c r="A55" s="104"/>
+      <c r="B55" s="128"/>
+      <c r="C55" s="126"/>
+      <c r="D55" s="178"/>
       <c r="E55" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F55" s="133"/>
-      <c r="G55" s="131"/>
+      <c r="F55" s="132"/>
+      <c r="G55" s="130"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="108"/>
-      <c r="B56" s="129"/>
-      <c r="C56" s="127"/>
-      <c r="D56" s="184"/>
+      <c r="A56" s="104"/>
+      <c r="B56" s="128"/>
+      <c r="C56" s="126"/>
+      <c r="D56" s="178"/>
       <c r="E56" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="F56" s="133"/>
-      <c r="G56" s="131"/>
+      <c r="F56" s="132"/>
+      <c r="G56" s="130"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="108"/>
-      <c r="B57" s="129"/>
-      <c r="C57" s="127"/>
-      <c r="D57" s="184"/>
+      <c r="A57" s="104"/>
+      <c r="B57" s="128"/>
+      <c r="C57" s="126"/>
+      <c r="D57" s="178"/>
       <c r="E57" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="F57" s="133"/>
-      <c r="G57" s="131"/>
+      <c r="F57" s="132"/>
+      <c r="G57" s="130"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="109"/>
-      <c r="B58" s="179"/>
-      <c r="C58" s="178"/>
-      <c r="D58" s="184"/>
+      <c r="A58" s="105"/>
+      <c r="B58" s="173"/>
+      <c r="C58" s="172"/>
+      <c r="D58" s="178"/>
       <c r="E58" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F58" s="176"/>
-      <c r="G58" s="177"/>
+      <c r="F58" s="170"/>
+      <c r="G58" s="171"/>
     </row>
     <row r="59" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="107" t="s">
+      <c r="A59" s="103" t="s">
         <v>130</v>
       </c>
       <c r="B59" s="34" t="s">
@@ -3886,7 +4103,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="108"/>
+      <c r="A60" s="104"/>
       <c r="B60" s="43" t="s">
         <v>136</v>
       </c>
@@ -3907,7 +4124,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A61" s="108"/>
+      <c r="A61" s="104"/>
       <c r="B61" s="38" t="s">
         <v>140</v>
       </c>
@@ -3928,7 +4145,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="108"/>
+      <c r="A62" s="104"/>
       <c r="B62" s="43" t="s">
         <v>145</v>
       </c>
@@ -3949,7 +4166,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="108"/>
+      <c r="A63" s="104"/>
       <c r="B63" s="38" t="s">
         <v>149</v>
       </c>
@@ -3970,7 +4187,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="108"/>
+      <c r="A64" s="104"/>
       <c r="B64" s="43" t="s">
         <v>219</v>
       </c>
@@ -3991,7 +4208,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="108"/>
+      <c r="A65" s="104"/>
       <c r="B65" s="38" t="s">
         <v>154</v>
       </c>
@@ -4012,7 +4229,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="108"/>
+      <c r="A66" s="104"/>
       <c r="B66" s="43" t="s">
         <v>155</v>
       </c>
@@ -4033,7 +4250,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="108"/>
+      <c r="A67" s="104"/>
       <c r="B67" s="38" t="s">
         <v>157</v>
       </c>
@@ -4054,7 +4271,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="109"/>
+      <c r="A68" s="105"/>
       <c r="B68" s="59" t="s">
         <v>162</v>
       </c>
@@ -4075,7 +4292,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="107" t="s">
+      <c r="A69" s="103" t="s">
         <v>164</v>
       </c>
       <c r="B69" s="17" t="s">
@@ -4098,7 +4315,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="108"/>
+      <c r="A70" s="104"/>
       <c r="B70" s="19" t="s">
         <v>166</v>
       </c>
@@ -4119,7 +4336,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="108"/>
+      <c r="A71" s="104"/>
       <c r="B71" s="18" t="s">
         <v>167</v>
       </c>
@@ -4140,11 +4357,11 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="108"/>
-      <c r="B72" s="112" t="s">
+      <c r="A72" s="104"/>
+      <c r="B72" s="108" t="s">
         <v>168</v>
       </c>
-      <c r="C72" s="110" t="s">
+      <c r="C72" s="106" t="s">
         <v>186</v>
       </c>
       <c r="D72" s="29" t="s">
@@ -4156,14 +4373,14 @@
       <c r="F72" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="G72" s="114" t="s">
+      <c r="G72" s="110" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="108"/>
-      <c r="B73" s="112"/>
-      <c r="C73" s="110"/>
+      <c r="A73" s="104"/>
+      <c r="B73" s="108"/>
+      <c r="C73" s="106"/>
       <c r="D73" s="29" t="s">
         <v>189</v>
       </c>
@@ -4173,12 +4390,12 @@
       <c r="F73" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="G73" s="115"/>
+      <c r="G73" s="111"/>
     </row>
     <row r="74" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="108"/>
-      <c r="B74" s="112"/>
-      <c r="C74" s="110"/>
+      <c r="A74" s="104"/>
+      <c r="B74" s="108"/>
+      <c r="C74" s="106"/>
       <c r="D74" s="29" t="s">
         <v>190</v>
       </c>
@@ -4188,12 +4405,12 @@
       <c r="F74" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="G74" s="115"/>
+      <c r="G74" s="111"/>
     </row>
     <row r="75" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="108"/>
-      <c r="B75" s="112"/>
-      <c r="C75" s="110"/>
+      <c r="A75" s="104"/>
+      <c r="B75" s="108"/>
+      <c r="C75" s="106"/>
       <c r="D75" s="29" t="s">
         <v>191</v>
       </c>
@@ -4203,12 +4420,12 @@
       <c r="F75" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="G75" s="115"/>
+      <c r="G75" s="111"/>
     </row>
     <row r="76" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="108"/>
-      <c r="B76" s="113"/>
-      <c r="C76" s="111"/>
+      <c r="A76" s="104"/>
+      <c r="B76" s="109"/>
+      <c r="C76" s="107"/>
       <c r="D76" s="57" t="s">
         <v>192</v>
       </c>
@@ -4218,10 +4435,10 @@
       <c r="F76" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="G76" s="116"/>
+      <c r="G76" s="112"/>
     </row>
     <row r="77" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="108"/>
+      <c r="A77" s="104"/>
       <c r="B77" s="69" t="s">
         <v>169</v>
       </c>
@@ -4242,7 +4459,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="108"/>
+      <c r="A78" s="104"/>
       <c r="B78" s="70" t="s">
         <v>170</v>
       </c>
@@ -4263,7 +4480,7 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A79" s="108"/>
+      <c r="A79" s="104"/>
       <c r="B79" s="71" t="s">
         <v>171</v>
       </c>
@@ -4284,7 +4501,7 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A80" s="108"/>
+      <c r="A80" s="104"/>
       <c r="B80" s="70" t="s">
         <v>172</v>
       </c>
@@ -4305,7 +4522,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A81" s="108"/>
+      <c r="A81" s="104"/>
       <c r="B81" s="71" t="s">
         <v>173</v>
       </c>
@@ -4326,7 +4543,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="108"/>
+      <c r="A82" s="104"/>
       <c r="B82" s="70" t="s">
         <v>174</v>
       </c>
@@ -4347,7 +4564,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A83" s="108"/>
+      <c r="A83" s="104"/>
       <c r="B83" s="71" t="s">
         <v>175</v>
       </c>
@@ -4368,7 +4585,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A84" s="108"/>
+      <c r="A84" s="104"/>
       <c r="B84" s="70" t="s">
         <v>176</v>
       </c>
@@ -4389,7 +4606,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A85" s="108"/>
+      <c r="A85" s="104"/>
       <c r="B85" s="71" t="s">
         <v>177</v>
       </c>
@@ -4410,7 +4627,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A86" s="108"/>
+      <c r="A86" s="104"/>
       <c r="B86" s="70" t="s">
         <v>178</v>
       </c>
@@ -4431,7 +4648,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="109"/>
+      <c r="A87" s="105"/>
       <c r="B87" s="75" t="s">
         <v>179</v>
       </c>
@@ -4452,7 +4669,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A88" s="174" t="s">
+      <c r="A88" s="190" t="s">
         <v>261</v>
       </c>
       <c r="B88" s="81" t="s">
@@ -4475,7 +4692,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="175"/>
+      <c r="A89" s="191"/>
       <c r="B89" s="18" t="s">
         <v>263</v>
       </c>
@@ -4496,7 +4713,7 @@
       </c>
     </row>
     <row r="90" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A90" s="175"/>
+      <c r="A90" s="191"/>
       <c r="B90" s="21" t="s">
         <v>264</v>
       </c>
@@ -4517,7 +4734,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A91" s="175"/>
+      <c r="A91" s="191"/>
       <c r="B91" s="18" t="s">
         <v>265</v>
       </c>
@@ -4538,7 +4755,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A92" s="175"/>
+      <c r="A92" s="191"/>
       <c r="B92" s="21" t="s">
         <v>266</v>
       </c>
@@ -4559,7 +4776,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="175"/>
+      <c r="A93" s="191"/>
       <c r="B93" s="18" t="s">
         <v>267</v>
       </c>
@@ -4580,7 +4797,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A94" s="175"/>
+      <c r="A94" s="191"/>
       <c r="B94" s="21" t="s">
         <v>268</v>
       </c>
@@ -4601,7 +4818,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A95" s="175"/>
+      <c r="A95" s="191"/>
       <c r="B95" s="18" t="s">
         <v>269</v>
       </c>
@@ -4622,7 +4839,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A96" s="175"/>
+      <c r="A96" s="191"/>
       <c r="B96" s="21" t="s">
         <v>270</v>
       </c>
@@ -4643,7 +4860,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A97" s="175"/>
+      <c r="A97" s="191"/>
       <c r="B97" s="18" t="s">
         <v>271</v>
       </c>
@@ -4664,7 +4881,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A98" s="175"/>
+      <c r="A98" s="191"/>
       <c r="B98" s="21" t="s">
         <v>272</v>
       </c>
@@ -4685,7 +4902,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A99" s="175"/>
+      <c r="A99" s="191"/>
       <c r="B99" s="18" t="s">
         <v>273</v>
       </c>
@@ -4706,7 +4923,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A100" s="175"/>
+      <c r="A100" s="191"/>
       <c r="B100" s="21" t="s">
         <v>274</v>
       </c>
@@ -4727,7 +4944,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A101" s="175"/>
+      <c r="A101" s="191"/>
       <c r="B101" s="18" t="s">
         <v>275</v>
       </c>
@@ -4748,7 +4965,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A102" s="175"/>
+      <c r="A102" s="191"/>
       <c r="B102" s="21" t="s">
         <v>276</v>
       </c>
@@ -4769,7 +4986,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A103" s="175"/>
+      <c r="A103" s="191"/>
       <c r="B103" s="18" t="s">
         <v>277</v>
       </c>
@@ -4790,7 +5007,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A104" s="175"/>
+      <c r="A104" s="191"/>
       <c r="B104" s="21" t="s">
         <v>278</v>
       </c>
@@ -4811,7 +5028,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A105" s="175"/>
+      <c r="A105" s="191"/>
       <c r="B105" s="18" t="s">
         <v>279</v>
       </c>
@@ -4832,7 +5049,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A106" s="175"/>
+      <c r="A106" s="191"/>
       <c r="B106" s="21" t="s">
         <v>280</v>
       </c>
@@ -4853,7 +5070,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A107" s="175"/>
+      <c r="A107" s="191"/>
       <c r="B107" s="18" t="s">
         <v>281</v>
       </c>
@@ -4874,7 +5091,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="175"/>
+      <c r="A108" s="191"/>
       <c r="B108" s="91" t="s">
         <v>282</v>
       </c>
@@ -4895,7 +5112,7 @@
       </c>
     </row>
     <row r="109" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A109" s="171" t="s">
+      <c r="A109" s="113" t="s">
         <v>374</v>
       </c>
       <c r="B109" s="17" t="s">
@@ -4918,7 +5135,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="172"/>
+      <c r="A110" s="114"/>
       <c r="B110" s="80" t="s">
         <v>376</v>
       </c>
@@ -4939,7 +5156,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A111" s="172"/>
+      <c r="A111" s="114"/>
       <c r="B111" s="18" t="s">
         <v>377</v>
       </c>
@@ -4960,11 +5177,11 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="173.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="172"/>
+      <c r="A112" s="114"/>
       <c r="B112" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="C112" s="99" t="s">
+      <c r="C112" s="96" t="s">
         <v>409</v>
       </c>
       <c r="D112" s="45" t="s">
@@ -4981,7 +5198,7 @@
       </c>
     </row>
     <row r="113" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="172"/>
+      <c r="A113" s="114"/>
       <c r="B113" s="18" t="s">
         <v>379</v>
       </c>
@@ -5002,7 +5219,7 @@
       </c>
     </row>
     <row r="114" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A114" s="172"/>
+      <c r="A114" s="114"/>
       <c r="B114" s="19" t="s">
         <v>380</v>
       </c>
@@ -5023,11 +5240,11 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="173.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="173"/>
+      <c r="A115" s="115"/>
       <c r="B115" s="90" t="s">
         <v>381</v>
       </c>
-      <c r="C115" s="100" t="s">
+      <c r="C115" s="97" t="s">
         <v>409</v>
       </c>
       <c r="D115" s="77" t="s">
@@ -5044,10 +5261,10 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A116" s="104" t="s">
+      <c r="A116" s="101" t="s">
         <v>415</v>
       </c>
-      <c r="B116" s="102" t="s">
+      <c r="B116" s="98" t="s">
         <v>416</v>
       </c>
       <c r="C116" s="82" t="s">
@@ -5067,7 +5284,7 @@
       </c>
     </row>
     <row r="117" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A117" s="105"/>
+      <c r="A117" s="102"/>
       <c r="B117" s="38" t="s">
         <v>417</v>
       </c>
@@ -5088,8 +5305,8 @@
       </c>
     </row>
     <row r="118" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A118" s="105"/>
-      <c r="B118" s="103" t="s">
+      <c r="A118" s="102"/>
+      <c r="B118" s="99" t="s">
         <v>418</v>
       </c>
       <c r="C118" s="86" t="s">
@@ -5109,7 +5326,7 @@
       </c>
     </row>
     <row r="119" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="105"/>
+      <c r="A119" s="102"/>
       <c r="B119" s="38" t="s">
         <v>419</v>
       </c>
@@ -5130,8 +5347,8 @@
       </c>
     </row>
     <row r="120" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A120" s="105"/>
-      <c r="B120" s="103" t="s">
+      <c r="A120" s="102"/>
+      <c r="B120" s="99" t="s">
         <v>420</v>
       </c>
       <c r="C120" s="86" t="s">
@@ -5151,7 +5368,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A121" s="105"/>
+      <c r="A121" s="102"/>
       <c r="B121" s="38" t="s">
         <v>421</v>
       </c>
@@ -5172,8 +5389,8 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A122" s="105"/>
-      <c r="B122" s="103" t="s">
+      <c r="A122" s="102"/>
+      <c r="B122" s="99" t="s">
         <v>422</v>
       </c>
       <c r="C122" s="86" t="s">
@@ -5193,28 +5410,112 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="106"/>
-      <c r="B123" s="101" t="s">
+      <c r="A123" s="179"/>
+      <c r="B123" s="180" t="s">
         <v>423</v>
       </c>
-      <c r="C123" s="96" t="s">
+      <c r="C123" s="97" t="s">
         <v>448</v>
       </c>
-      <c r="D123" s="97" t="s">
+      <c r="D123" s="77" t="s">
         <v>459</v>
       </c>
-      <c r="E123" s="97" t="s">
+      <c r="E123" s="77" t="s">
         <v>450</v>
       </c>
-      <c r="F123" s="98" t="s">
+      <c r="F123" s="78" t="s">
         <v>457</v>
       </c>
-      <c r="G123" s="185" t="s">
+      <c r="G123" s="79" t="s">
         <v>458</v>
       </c>
     </row>
+    <row r="124" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A124" s="103" t="s">
+        <v>460</v>
+      </c>
+      <c r="B124" s="181" t="s">
+        <v>461</v>
+      </c>
+      <c r="C124" s="182"/>
+      <c r="D124" s="183"/>
+      <c r="E124" s="183"/>
+      <c r="F124" s="184" t="s">
+        <v>468</v>
+      </c>
+      <c r="G124" s="184"/>
+    </row>
+    <row r="125" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A125" s="104"/>
+      <c r="B125" s="186" t="s">
+        <v>462</v>
+      </c>
+      <c r="C125" s="187"/>
+      <c r="D125" s="188"/>
+      <c r="E125" s="188"/>
+      <c r="F125" s="189" t="s">
+        <v>469</v>
+      </c>
+      <c r="G125" s="189"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A126" s="104"/>
+      <c r="B126" s="43" t="s">
+        <v>463</v>
+      </c>
+      <c r="C126" s="47"/>
+      <c r="D126" s="45"/>
+      <c r="E126" s="45"/>
+      <c r="F126" s="46"/>
+      <c r="G126" s="46"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A127" s="104"/>
+      <c r="B127" s="186" t="s">
+        <v>464</v>
+      </c>
+      <c r="C127" s="187"/>
+      <c r="D127" s="188"/>
+      <c r="E127" s="188"/>
+      <c r="F127" s="189"/>
+      <c r="G127" s="189"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128" s="104"/>
+      <c r="B128" s="43" t="s">
+        <v>466</v>
+      </c>
+      <c r="C128" s="47"/>
+      <c r="D128" s="45"/>
+      <c r="E128" s="45"/>
+      <c r="F128" s="46"/>
+      <c r="G128" s="46"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129" s="104"/>
+      <c r="B129" s="186" t="s">
+        <v>467</v>
+      </c>
+      <c r="C129" s="187"/>
+      <c r="D129" s="188"/>
+      <c r="E129" s="188"/>
+      <c r="F129" s="189"/>
+      <c r="G129" s="189"/>
+    </row>
+    <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="116"/>
+      <c r="B130" s="185" t="s">
+        <v>465</v>
+      </c>
+      <c r="C130" s="96"/>
+      <c r="D130" s="100"/>
+      <c r="E130" s="100"/>
+      <c r="F130" s="48"/>
+      <c r="G130" s="48"/>
+    </row>
   </sheetData>
-  <mergeCells count="62">
+  <mergeCells count="63">
+    <mergeCell ref="A124:A130"/>
     <mergeCell ref="A59:A68"/>
     <mergeCell ref="F50:F58"/>
     <mergeCell ref="G50:G58"/>
@@ -5359,4 +5660,187 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId77"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC374DC0-6B38-44DC-990C-3E2EEBDDFA20}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="3" width="37.44140625" style="192" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" style="206" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" style="206" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" style="206" customWidth="1"/>
+    <col min="7" max="7" width="51.109375" style="206" customWidth="1"/>
+    <col min="8" max="8" width="65" style="206" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="137" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="139"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="140"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="142"/>
+    </row>
+    <row r="3" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="193" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="194" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="195" t="s">
+        <v>475</v>
+      </c>
+      <c r="D3" s="196" t="s">
+        <v>319</v>
+      </c>
+      <c r="E3" s="194" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="196" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="196" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="214" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="198" t="s">
+        <v>476</v>
+      </c>
+      <c r="C4" s="197" t="s">
+        <v>477</v>
+      </c>
+      <c r="D4" s="202" t="s">
+        <v>478</v>
+      </c>
+      <c r="E4" s="202" t="s">
+        <v>479</v>
+      </c>
+      <c r="F4" s="202" t="s">
+        <v>480</v>
+      </c>
+      <c r="G4" s="209" t="s">
+        <v>481</v>
+      </c>
+      <c r="H4" s="209" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="104"/>
+      <c r="B5" s="199" t="s">
+        <v>483</v>
+      </c>
+      <c r="C5" s="199" t="s">
+        <v>485</v>
+      </c>
+      <c r="D5" s="203" t="s">
+        <v>484</v>
+      </c>
+      <c r="E5" s="203" t="s">
+        <v>486</v>
+      </c>
+      <c r="F5" s="203" t="s">
+        <v>487</v>
+      </c>
+      <c r="G5" s="210" t="s">
+        <v>488</v>
+      </c>
+      <c r="H5" s="211" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="104"/>
+      <c r="B6" s="200" t="s">
+        <v>470</v>
+      </c>
+      <c r="C6" s="200" t="s">
+        <v>471</v>
+      </c>
+      <c r="D6" s="204" t="s">
+        <v>490</v>
+      </c>
+      <c r="E6" s="204" t="s">
+        <v>489</v>
+      </c>
+      <c r="F6" s="208" t="s">
+        <v>491</v>
+      </c>
+      <c r="G6" s="212" t="s">
+        <v>474</v>
+      </c>
+      <c r="H6" s="212" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="116"/>
+      <c r="B7" s="201" t="s">
+        <v>492</v>
+      </c>
+      <c r="C7" s="201" t="s">
+        <v>495</v>
+      </c>
+      <c r="D7" s="205" t="s">
+        <v>493</v>
+      </c>
+      <c r="E7" s="207" t="s">
+        <v>497</v>
+      </c>
+      <c r="F7" s="205" t="s">
+        <v>498</v>
+      </c>
+      <c r="G7" s="213" t="s">
+        <v>494</v>
+      </c>
+      <c r="H7" s="213" t="s">
+        <v>496</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A4:A7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1" location="L28" xr:uid="{B04D7226-E4C4-4E3A-B827-04DBB55FE032}"/>
+    <hyperlink ref="G6" r:id="rId2" location="L58" xr:uid="{837C92EE-22AF-4058-B18C-1728F1BA8EB7}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{D44B8646-47EA-420C-86AF-0EEB8F5BCFA0}"/>
+    <hyperlink ref="H4" r:id="rId4" location="L4" xr:uid="{A1715482-93CF-4E16-A269-1E28A4D4075E}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{DBF175BB-DB92-435B-BA52-F606543B824A}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{7C83257E-FE5C-4816-94B0-A7876AC5655C}"/>
+    <hyperlink ref="H7" r:id="rId7" location="L27" xr:uid="{09E0F68D-20AE-49F1-9CDE-11B7767C3377}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>